<commit_message>
Add CFs for specific CO2 flows to account for NETs
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904404BE-FB7F-412E-9C87-0C9FABB7F5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A750769-C31F-4BAF-A30A-8C10C605C71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$84</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -274,6 +277,27 @@
   </si>
   <si>
     <t>air::urban air close to ground</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, in air</t>
+  </si>
+  <si>
+    <t>natural resource::in air</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, non-fossil, resource correction</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, non-fossil</t>
+  </si>
+  <si>
+    <t>air::lower stratosphere + upper troposphere</t>
+  </si>
+  <si>
+    <t>air::non-urban air or from high stacks</t>
+  </si>
+  <si>
+    <t>air::unspecified</t>
   </si>
 </sst>
 </file>
@@ -600,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,6 +1484,83 @@
         <v>5.418069230769231E-9</v>
       </c>
     </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78">
+        <v>-2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79">
+        <v>-2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Get GW component of CBI directly from simapro
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904404BE-FB7F-412E-9C87-0C9FABB7F5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC4FBFB-BDAB-4FCF-BA34-EB1D77D18328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="86">
   <si>
     <t>name</t>
   </si>
@@ -156,124 +156,133 @@
     <t>Hydrocarbons, chlorinated</t>
   </si>
   <si>
-    <t>carbon dioxide, fossil</t>
-  </si>
-  <si>
-    <t>carbon dioxide, from soil or biomass stock</t>
-  </si>
-  <si>
-    <t>carbon dioxide, to soil or biomass stock</t>
-  </si>
-  <si>
-    <t>soil</t>
-  </si>
-  <si>
-    <t>dinitrogen monoxide</t>
-  </si>
-  <si>
-    <t>ethane, 1,1,1,2-tetrafluoro-, hfc-134a</t>
-  </si>
-  <si>
-    <t>ethane, 1,1,1-trifluoro-, hfc-143a</t>
-  </si>
-  <si>
-    <t>ethane, 1,1,2-trichloro-1,2,2-trifluoro-, cfc-113</t>
-  </si>
-  <si>
-    <t>ethane, 1,1-dichloro-1-fluoro-, hcfc-141b</t>
-  </si>
-  <si>
-    <t>ethane, 1,1-difluoro-, hfc-152a</t>
-  </si>
-  <si>
-    <t>ethane, 1,2-dichloro-1,1,2,2-tetrafluoro-, cfc-114</t>
-  </si>
-  <si>
-    <t>ethane, 1-chloro-1,1-difluoro-, hcfc-142b</t>
-  </si>
-  <si>
-    <t>ethane, 2,2-dichloro-1,1,1-trifluoro-, hcfc-123</t>
-  </si>
-  <si>
-    <t>ethane, 2-chloro-1,1,1,2-tetrafluoro-, hcfc-124</t>
-  </si>
-  <si>
-    <t>ethane, chloropentafluoro-, cfc-115</t>
-  </si>
-  <si>
-    <t>ethane, hexafluoro-, hfc-116</t>
-  </si>
-  <si>
-    <t>ethane, pentafluoro-, hfc-125</t>
-  </si>
-  <si>
-    <t>methane, bromo-, halon 1001</t>
-  </si>
-  <si>
-    <t>methane, bromochlorodifluoro-, halon 1211</t>
-  </si>
-  <si>
-    <t>methane, bromotrifluoro-, halon 1301</t>
-  </si>
-  <si>
-    <t>methane, chlorodifluoro-, hcfc-22</t>
-  </si>
-  <si>
-    <t>methane, chlorotrifluoro-, cfc-13</t>
-  </si>
-  <si>
-    <t>methane, dichloro-, hcc-30</t>
-  </si>
-  <si>
-    <t>methane, dichlorodifluoro-, cfc-12</t>
-  </si>
-  <si>
-    <t>methane, dichlorofluoro-, hcfc-21</t>
-  </si>
-  <si>
-    <t>methane, difluoro-, hfc-32</t>
-  </si>
-  <si>
-    <t>methane, fossil</t>
-  </si>
-  <si>
-    <t>methane, from soil or biomass stock</t>
-  </si>
-  <si>
-    <t>methane, monochloro-, r-40</t>
-  </si>
-  <si>
-    <t>methane, non-fossil</t>
-  </si>
-  <si>
-    <t>methane, tetrachloro-, r-10</t>
-  </si>
-  <si>
-    <t>methane, tetrafluoro-, r-14</t>
-  </si>
-  <si>
-    <t>methane, trichlorofluoro-, cfc-11</t>
-  </si>
-  <si>
-    <t>methane, trifluoro-, hfc-23</t>
-  </si>
-  <si>
-    <t>nitrogen fluoride</t>
-  </si>
-  <si>
-    <t>perfluoropentane</t>
-  </si>
-  <si>
-    <t>sulfur hexafluoride</t>
-  </si>
-  <si>
     <t>natural resource::land</t>
   </si>
   <si>
-    <t>methane</t>
-  </si>
-  <si>
-    <t>air::urban air close to ground</t>
+    <t>Carbon dioxide, fossil</t>
+  </si>
+  <si>
+    <t>air:low population density, long-term</t>
+  </si>
+  <si>
+    <t>air:lower stratosphere + upper troposphere</t>
+  </si>
+  <si>
+    <t>air:non-urban air or from high stacks</t>
+  </si>
+  <si>
+    <t>air:urban air close to ground</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, from soil or biomass stock</t>
+  </si>
+  <si>
+    <t>air:indoor</t>
+  </si>
+  <si>
+    <t>Dinitrogen monoxide</t>
+  </si>
+  <si>
+    <t>Ethane, 1,1,1,2-tetrafluoro-, HFC-134a</t>
+  </si>
+  <si>
+    <t>Ethane, 1,1,1-trichloro-, HCFC-140</t>
+  </si>
+  <si>
+    <t>Ethane, 1,1,1-trifluoro-, HFC-143a</t>
+  </si>
+  <si>
+    <t>Ethane, 1,1,2-trichloro-1,2,2-trifluoro-, CFC-113</t>
+  </si>
+  <si>
+    <t>Ethane, 1,1-dichloro-1-fluoro-, HCFC-141b</t>
+  </si>
+  <si>
+    <t>Ethane, 1,1-difluoro-, HFC-152a</t>
+  </si>
+  <si>
+    <t>Ethane, 1,2-dichloro-</t>
+  </si>
+  <si>
+    <t>Ethane, 1,2-dichloro-1,1,2,2-tetrafluoro-, CFC-114</t>
+  </si>
+  <si>
+    <t>Ethane, 1-chloro-1,1-difluoro-, HCFC-142b</t>
+  </si>
+  <si>
+    <t>Ethane, 2,2-dichloro-1,1,1-trifluoro-, HCFC-123</t>
+  </si>
+  <si>
+    <t>Ethane, 2-chloro-1,1,1,2-tetrafluoro-, HCFC-124</t>
+  </si>
+  <si>
+    <t>Ethane, chloropentafluoro-, CFC-115</t>
+  </si>
+  <si>
+    <t>Ethane, hexafluoro-, HFC-116</t>
+  </si>
+  <si>
+    <t>Ethane, pentafluoro-, HFC-125</t>
+  </si>
+  <si>
+    <t>Methane</t>
+  </si>
+  <si>
+    <t>Methane, bromo-, Halon 1001</t>
+  </si>
+  <si>
+    <t>Methane, bromochlorodifluoro-, Halon 1211</t>
+  </si>
+  <si>
+    <t>Methane, bromotrifluoro-, Halon 1301</t>
+  </si>
+  <si>
+    <t>Methane, chlorodifluoro-, HCFC-22</t>
+  </si>
+  <si>
+    <t>Methane, chlorotrifluoro-, CFC-13</t>
+  </si>
+  <si>
+    <t>Methane, dichloro-, HCC-30</t>
+  </si>
+  <si>
+    <t>Methane, dichlorodifluoro-, CFC-12</t>
+  </si>
+  <si>
+    <t>Methane, dichlorofluoro-, HCFC-21</t>
+  </si>
+  <si>
+    <t>Methane, difluoro-, HFC-32</t>
+  </si>
+  <si>
+    <t>Methane, fossil</t>
+  </si>
+  <si>
+    <t>Methane, from soil or biomass stock</t>
+  </si>
+  <si>
+    <t>Methane, monochloro-, R-40</t>
+  </si>
+  <si>
+    <t>Methane, non-fossil</t>
+  </si>
+  <si>
+    <t>Methane, tetrachloro-, R-10</t>
+  </si>
+  <si>
+    <t>Methane, tetrafluoro-, R-14</t>
+  </si>
+  <si>
+    <t>Methane, trichlorofluoro-, CFC-11</t>
+  </si>
+  <si>
+    <t>Methane, trifluoro-, HFC-23</t>
+  </si>
+  <si>
+    <t>Nitrogen fluoride</t>
+  </si>
+  <si>
+    <t>Sulfur hexafluoride</t>
   </si>
 </sst>
 </file>
@@ -600,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>6.9230769230769235E-13</v>
@@ -640,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>6.9230769230769235E-13</v>
@@ -651,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>6.9230769230769235E-13</v>
@@ -662,7 +671,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>5.3846153846153838E-13</v>
@@ -673,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>6.9230769230769235E-13</v>
@@ -684,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>6.9230769230769235E-13</v>
@@ -695,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>5.3846153846153838E-13</v>
@@ -706,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>6.9230769230769235E-13</v>
@@ -717,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>6.9230769230769235E-13</v>
@@ -728,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>7.3076923076923074E-13</v>
@@ -739,7 +748,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>7.3076923076923074E-13</v>
@@ -750,7 +759,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C13">
         <v>2.307692307692307E-13</v>
@@ -761,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>6.1538461538461536E-13</v>
@@ -772,7 +781,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <v>3.8461538461538462E-13</v>
@@ -783,7 +792,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>3.8461538461538462E-13</v>
@@ -794,7 +803,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>3.8461538461538462E-13</v>
@@ -805,7 +814,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C18">
         <v>7.3076923076923074E-13</v>
@@ -816,7 +825,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>7.3076923076923074E-13</v>
@@ -827,7 +836,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>6.9230769230769235E-13</v>
@@ -838,7 +847,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>2.307692307692307E-13</v>
@@ -849,7 +858,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>6.9230769230769235E-13</v>
@@ -860,7 +869,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>6.9230769230769235E-13</v>
@@ -871,7 +880,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>6.9230769230769235E-13</v>
@@ -882,7 +891,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>5.3846153846153838E-13</v>
@@ -893,7 +902,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>6.9230769230769235E-13</v>
@@ -904,7 +913,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>6.9230769230769235E-13</v>
@@ -915,7 +924,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>5.3846153846153838E-13</v>
@@ -926,7 +935,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>6.9230769230769235E-13</v>
@@ -937,7 +946,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>7.6923076923076923E-13</v>
@@ -948,7 +957,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -959,7 +968,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>7.3076923076923074E-13</v>
@@ -970,7 +979,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>7.3076923076923074E-13</v>
@@ -981,7 +990,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C34">
         <v>7.3076923076923074E-13</v>
@@ -992,7 +1001,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>7.3076923076923074E-13</v>
@@ -1003,7 +1012,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>7.3076923076923074E-13</v>
@@ -1014,7 +1023,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <v>7.3076923076923074E-13</v>
@@ -1025,7 +1034,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>7.3076923076923074E-13</v>
@@ -1033,32 +1042,32 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
       </c>
       <c r="C39">
-        <v>4.1538461538461543E-12</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C40">
-        <v>2.8661538461538461E-12</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>2.076923076923077E-13</v>
@@ -1069,7 +1078,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>2.076923076923077E-13</v>
@@ -1077,35 +1086,35 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C43">
-        <v>-2.076923076923077E-13</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
       </c>
       <c r="C44">
-        <v>6.1892307692307702E-11</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C45">
-        <v>3.2171538461538461E-10</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1113,351 +1122,2045 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C46">
-        <v>1.143969230769231E-9</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C47">
-        <v>1.3678615384615381E-9</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C48">
-        <v>1.9481538461538459E-10</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C49">
-        <v>3.4684615384615383E-11</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
       </c>
       <c r="C50">
-        <v>1.9969615384615379E-9</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C51">
-        <v>4.8703846153846161E-10</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C52">
-        <v>1.9938461538461541E-11</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C53">
-        <v>1.3188461538461541E-10</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C54">
-        <v>1.7687076923076921E-9</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>41</v>
       </c>
       <c r="C55">
-        <v>2.5629230769230769E-9</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C56">
-        <v>7.6659230769230773E-10</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C57">
-        <v>7.4769230769230768E-12</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C58">
-        <v>6.2307692307692306E-13</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C59">
-        <v>4.29923076923077E-10</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
       </c>
       <c r="C60">
-        <v>1.4858307692307699E-9</v>
+        <v>3.2192307692307691E-10</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C61">
-        <v>4.3740000000000001E-10</v>
+        <v>3.2192307692307691E-10</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C62">
-        <v>3.2090538461538469E-9</v>
+        <v>3.2192307692307691E-10</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C63">
-        <v>2.2846153846153851E-12</v>
+        <v>3.2192307692307691E-10</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C64">
-        <v>2.3982230769230768E-9</v>
+        <v>3.2192307692307691E-10</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
         <v>41</v>
       </c>
       <c r="C65">
-        <v>3.7176923076923081E-11</v>
+        <v>4.0084615384615378E-11</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C66">
-        <v>1.6968461538461539E-10</v>
+        <v>4.0084615384615378E-11</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C67">
-        <v>7.4769230769230768E-12</v>
+        <v>4.0084615384615378E-11</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C68">
-        <v>7.0615384615384616E-12</v>
+        <v>4.0084615384615378E-11</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C69">
-        <v>3.1153846153846161E-12</v>
+        <v>4.0084615384615378E-11</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B70" t="s">
         <v>41</v>
       </c>
       <c r="C70">
-        <v>7.0615384615384616E-12</v>
+        <v>1.1443846153846149E-9</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C71">
-        <v>4.1933076923076919E-10</v>
+        <v>1.1443846153846149E-9</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C72">
-        <v>1.5263307692307689E-9</v>
+        <v>1.1443846153846149E-9</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C73">
-        <v>1.111569230769231E-9</v>
+        <v>1.1443846153846149E-9</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C74">
-        <v>2.8777846153846162E-9</v>
+        <v>1.1443846153846149E-9</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B75" t="s">
         <v>41</v>
       </c>
       <c r="C75">
-        <v>3.714576923076923E-9</v>
+        <v>1.3686923076923081E-9</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C76">
-        <v>1.969753846153846E-9</v>
+        <v>1.3686923076923081E-9</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77" t="s">
+        <v>46</v>
+      </c>
+      <c r="C77">
+        <v>1.3686923076923081E-9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78">
+        <v>1.3686923076923081E-9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79">
+        <v>1.3686923076923081E-9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>56</v>
+      </c>
+      <c r="B80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C80">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" t="s">
+        <v>45</v>
+      </c>
+      <c r="C81">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>56</v>
+      </c>
+      <c r="B84" t="s">
+        <v>48</v>
+      </c>
+      <c r="C84">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85" t="s">
+        <v>41</v>
+      </c>
+      <c r="C85">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87" t="s">
+        <v>46</v>
+      </c>
+      <c r="C87">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88" t="s">
+        <v>47</v>
+      </c>
+      <c r="C88">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>57</v>
+      </c>
+      <c r="B89" t="s">
+        <v>48</v>
+      </c>
+      <c r="C89">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>58</v>
+      </c>
+      <c r="B90" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>58</v>
+      </c>
+      <c r="B91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>58</v>
+      </c>
+      <c r="B92" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>58</v>
+      </c>
+      <c r="B93" t="s">
+        <v>47</v>
+      </c>
+      <c r="C93">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>58</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94">
+        <v>2.076923076923077E-13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>59</v>
+      </c>
+      <c r="B95" t="s">
+        <v>41</v>
+      </c>
+      <c r="C95">
+        <v>1.9979999999999999E-9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96">
+        <v>1.9979999999999999E-9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>59</v>
+      </c>
+      <c r="B97" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97">
+        <v>1.9979999999999999E-9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+      <c r="B98" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98">
+        <v>1.9979999999999999E-9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B99" t="s">
+        <v>48</v>
+      </c>
+      <c r="C99">
+        <v>1.9979999999999999E-9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>60</v>
+      </c>
+      <c r="B100" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100">
+        <v>4.8807692307692314E-10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>60</v>
+      </c>
+      <c r="B101" t="s">
+        <v>45</v>
+      </c>
+      <c r="C101">
+        <v>4.8807692307692314E-10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>60</v>
+      </c>
+      <c r="B102" t="s">
+        <v>46</v>
+      </c>
+      <c r="C102">
+        <v>4.8807692307692314E-10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>60</v>
+      </c>
+      <c r="B103" t="s">
+        <v>47</v>
+      </c>
+      <c r="C103">
+        <v>4.8807692307692314E-10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>60</v>
+      </c>
+      <c r="B104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C104">
+        <v>4.8807692307692314E-10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" t="s">
+        <v>41</v>
+      </c>
+      <c r="C105">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>61</v>
+      </c>
+      <c r="B106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C106">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>61</v>
+      </c>
+      <c r="B107" t="s">
+        <v>46</v>
+      </c>
+      <c r="C107">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>61</v>
+      </c>
+      <c r="B108" t="s">
+        <v>47</v>
+      </c>
+      <c r="C108">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>61</v>
+      </c>
+      <c r="B109" t="s">
+        <v>48</v>
+      </c>
+      <c r="C109">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>62</v>
+      </c>
+      <c r="B110" t="s">
+        <v>41</v>
+      </c>
+      <c r="C110">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>62</v>
+      </c>
+      <c r="B111" t="s">
+        <v>45</v>
+      </c>
+      <c r="C111">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>62</v>
+      </c>
+      <c r="B112" t="s">
+        <v>46</v>
+      </c>
+      <c r="C112">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>62</v>
+      </c>
+      <c r="B113" t="s">
+        <v>47</v>
+      </c>
+      <c r="C113">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>62</v>
+      </c>
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>63</v>
+      </c>
+      <c r="B115" t="s">
+        <v>41</v>
+      </c>
+      <c r="C115">
+        <v>1.7695384615384611E-9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>63</v>
+      </c>
+      <c r="B116" t="s">
+        <v>45</v>
+      </c>
+      <c r="C116">
+        <v>1.7695384615384611E-9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>63</v>
+      </c>
+      <c r="B117" t="s">
+        <v>46</v>
+      </c>
+      <c r="C117">
+        <v>1.7695384615384611E-9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>63</v>
+      </c>
+      <c r="B118" t="s">
+        <v>47</v>
+      </c>
+      <c r="C118">
+        <v>1.7695384615384611E-9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>63</v>
+      </c>
+      <c r="B119" t="s">
+        <v>48</v>
+      </c>
+      <c r="C119">
+        <v>1.7695384615384611E-9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>64</v>
+      </c>
+      <c r="B120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C120">
+        <v>2.554615384615385E-9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>64</v>
+      </c>
+      <c r="B121" t="s">
+        <v>45</v>
+      </c>
+      <c r="C121">
+        <v>2.554615384615385E-9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>64</v>
+      </c>
+      <c r="B122" t="s">
+        <v>46</v>
+      </c>
+      <c r="C122">
+        <v>2.554615384615385E-9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" t="s">
+        <v>47</v>
+      </c>
+      <c r="C123">
+        <v>2.554615384615385E-9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>64</v>
+      </c>
+      <c r="B124" t="s">
+        <v>48</v>
+      </c>
+      <c r="C124">
+        <v>2.554615384615385E-9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>65</v>
+      </c>
+      <c r="B125" t="s">
+        <v>41</v>
+      </c>
+      <c r="C125">
+        <v>7.6638461538461539E-10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>65</v>
+      </c>
+      <c r="B126" t="s">
+        <v>45</v>
+      </c>
+      <c r="C126">
+        <v>7.6638461538461539E-10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>65</v>
+      </c>
+      <c r="B127" t="s">
+        <v>46</v>
+      </c>
+      <c r="C127">
+        <v>7.6638461538461539E-10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>65</v>
+      </c>
+      <c r="B128" t="s">
+        <v>47</v>
+      </c>
+      <c r="C128">
+        <v>7.6638461538461539E-10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>65</v>
+      </c>
+      <c r="B129" t="s">
+        <v>48</v>
+      </c>
+      <c r="C129">
+        <v>7.6638461538461539E-10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>42</v>
+      </c>
+      <c r="B130" t="s">
+        <v>41</v>
+      </c>
+      <c r="C130">
+        <v>2.8661538461538461E-12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>42</v>
+      </c>
+      <c r="B131" t="s">
+        <v>45</v>
+      </c>
+      <c r="C131">
+        <v>2.8661538461538461E-12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>42</v>
+      </c>
+      <c r="B132" t="s">
+        <v>46</v>
+      </c>
+      <c r="C132">
+        <v>2.8661538461538461E-12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>42</v>
+      </c>
+      <c r="B133" t="s">
+        <v>47</v>
+      </c>
+      <c r="C133">
+        <v>2.8661538461538461E-12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>42</v>
+      </c>
+      <c r="B134" t="s">
+        <v>48</v>
+      </c>
+      <c r="C134">
+        <v>2.8661538461538461E-12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>66</v>
+      </c>
+      <c r="B135" t="s">
+        <v>48</v>
+      </c>
+      <c r="C135">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>67</v>
+      </c>
+      <c r="B136" t="s">
+        <v>41</v>
+      </c>
+      <c r="C136">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>67</v>
+      </c>
+      <c r="B137" t="s">
+        <v>45</v>
+      </c>
+      <c r="C137">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>67</v>
+      </c>
+      <c r="B138" t="s">
+        <v>46</v>
+      </c>
+      <c r="C138">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>67</v>
+      </c>
+      <c r="B139" t="s">
+        <v>47</v>
+      </c>
+      <c r="C139">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>67</v>
+      </c>
+      <c r="B140" t="s">
+        <v>48</v>
+      </c>
+      <c r="C140">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>68</v>
+      </c>
+      <c r="B141" t="s">
+        <v>41</v>
+      </c>
+      <c r="C141">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>68</v>
+      </c>
+      <c r="B142" t="s">
+        <v>45</v>
+      </c>
+      <c r="C142">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>68</v>
+      </c>
+      <c r="B143" t="s">
+        <v>46</v>
+      </c>
+      <c r="C143">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>68</v>
+      </c>
+      <c r="B144" t="s">
+        <v>47</v>
+      </c>
+      <c r="C144">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>68</v>
+      </c>
+      <c r="B145" t="s">
+        <v>48</v>
+      </c>
+      <c r="C145">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>69</v>
+      </c>
+      <c r="B146" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146">
+        <v>1.4849999999999999E-9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>69</v>
+      </c>
+      <c r="B147" t="s">
+        <v>45</v>
+      </c>
+      <c r="C147">
+        <v>1.4849999999999999E-9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>69</v>
+      </c>
+      <c r="B148" t="s">
+        <v>46</v>
+      </c>
+      <c r="C148">
+        <v>1.4849999999999999E-9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>69</v>
+      </c>
+      <c r="B149" t="s">
+        <v>47</v>
+      </c>
+      <c r="C149">
+        <v>1.4849999999999999E-9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>69</v>
+      </c>
+      <c r="B150" t="s">
+        <v>48</v>
+      </c>
+      <c r="C150">
+        <v>1.4849999999999999E-9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>70</v>
+      </c>
+      <c r="B151" t="s">
+        <v>41</v>
+      </c>
+      <c r="C151">
+        <v>4.3823076923076919E-10</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>70</v>
+      </c>
+      <c r="B152" t="s">
+        <v>45</v>
+      </c>
+      <c r="C152">
+        <v>4.3823076923076919E-10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>70</v>
+      </c>
+      <c r="B153" t="s">
+        <v>46</v>
+      </c>
+      <c r="C153">
+        <v>4.3823076923076919E-10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>70</v>
+      </c>
+      <c r="B154" t="s">
+        <v>47</v>
+      </c>
+      <c r="C154">
+        <v>4.3823076923076919E-10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>70</v>
+      </c>
+      <c r="B155" t="s">
+        <v>48</v>
+      </c>
+      <c r="C155">
+        <v>4.3823076923076919E-10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>71</v>
+      </c>
+      <c r="B156" t="s">
+        <v>41</v>
+      </c>
+      <c r="C156">
+        <v>3.2192307692307689E-9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>71</v>
+      </c>
+      <c r="B157" t="s">
+        <v>45</v>
+      </c>
+      <c r="C157">
+        <v>3.2192307692307689E-9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>71</v>
+      </c>
+      <c r="B158" t="s">
+        <v>46</v>
+      </c>
+      <c r="C158">
+        <v>3.2192307692307689E-9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>71</v>
+      </c>
+      <c r="B159" t="s">
+        <v>47</v>
+      </c>
+      <c r="C159">
+        <v>3.2192307692307689E-9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>71</v>
+      </c>
+      <c r="B160" t="s">
+        <v>48</v>
+      </c>
+      <c r="C160">
+        <v>3.2192307692307689E-9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>72</v>
+      </c>
+      <c r="B161" t="s">
+        <v>41</v>
+      </c>
+      <c r="C161">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>72</v>
+      </c>
+      <c r="B162" t="s">
+        <v>45</v>
+      </c>
+      <c r="C162">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>72</v>
+      </c>
+      <c r="B163" t="s">
+        <v>46</v>
+      </c>
+      <c r="C163">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>72</v>
+      </c>
+      <c r="B164" t="s">
+        <v>47</v>
+      </c>
+      <c r="C164">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>72</v>
+      </c>
+      <c r="B165" t="s">
+        <v>48</v>
+      </c>
+      <c r="C165">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>73</v>
+      </c>
+      <c r="B166" t="s">
+        <v>41</v>
+      </c>
+      <c r="C166">
+        <v>2.388461538461538E-9</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>73</v>
+      </c>
+      <c r="B167" t="s">
+        <v>45</v>
+      </c>
+      <c r="C167">
+        <v>2.388461538461538E-9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>73</v>
+      </c>
+      <c r="B168" t="s">
+        <v>46</v>
+      </c>
+      <c r="C168">
+        <v>2.388461538461538E-9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>73</v>
+      </c>
+      <c r="B169" t="s">
+        <v>47</v>
+      </c>
+      <c r="C169">
+        <v>2.388461538461538E-9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>73</v>
+      </c>
+      <c r="B170" t="s">
+        <v>48</v>
+      </c>
+      <c r="C170">
+        <v>2.388461538461538E-9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>74</v>
+      </c>
+      <c r="B171" t="s">
+        <v>41</v>
+      </c>
+      <c r="C171">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>74</v>
+      </c>
+      <c r="B172" t="s">
+        <v>45</v>
+      </c>
+      <c r="C172">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>74</v>
+      </c>
+      <c r="B173" t="s">
+        <v>46</v>
+      </c>
+      <c r="C173">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>74</v>
+      </c>
+      <c r="B174" t="s">
+        <v>47</v>
+      </c>
+      <c r="C174">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>74</v>
+      </c>
+      <c r="B175" t="s">
+        <v>48</v>
+      </c>
+      <c r="C175">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>75</v>
+      </c>
+      <c r="B176" t="s">
+        <v>41</v>
+      </c>
+      <c r="C176">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>75</v>
+      </c>
+      <c r="B177" t="s">
+        <v>45</v>
+      </c>
+      <c r="C177">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>75</v>
+      </c>
+      <c r="B178" t="s">
+        <v>46</v>
+      </c>
+      <c r="C178">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>75</v>
+      </c>
+      <c r="B179" t="s">
+        <v>47</v>
+      </c>
+      <c r="C179">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>75</v>
+      </c>
+      <c r="B180" t="s">
+        <v>48</v>
+      </c>
+      <c r="C180">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>76</v>
+      </c>
+      <c r="B181" t="s">
+        <v>41</v>
+      </c>
+      <c r="C181">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>76</v>
+      </c>
+      <c r="B182" t="s">
+        <v>45</v>
+      </c>
+      <c r="C182">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>76</v>
+      </c>
+      <c r="B183" t="s">
+        <v>46</v>
+      </c>
+      <c r="C183">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>76</v>
+      </c>
+      <c r="B184" t="s">
+        <v>47</v>
+      </c>
+      <c r="C184">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>76</v>
+      </c>
+      <c r="B185" t="s">
+        <v>48</v>
+      </c>
+      <c r="C185">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>77</v>
+      </c>
+      <c r="B186" t="s">
+        <v>41</v>
+      </c>
+      <c r="C186">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>77</v>
+      </c>
+      <c r="B187" t="s">
+        <v>50</v>
+      </c>
+      <c r="C187">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>77</v>
+      </c>
+      <c r="B188" t="s">
+        <v>45</v>
+      </c>
+      <c r="C188">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>77</v>
+      </c>
+      <c r="B189" t="s">
+        <v>46</v>
+      </c>
+      <c r="C189">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>77</v>
+      </c>
+      <c r="B190" t="s">
+        <v>47</v>
+      </c>
+      <c r="C190">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>77</v>
+      </c>
+      <c r="B191" t="s">
+        <v>48</v>
+      </c>
+      <c r="C191">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>78</v>
+      </c>
+      <c r="B192" t="s">
+        <v>41</v>
+      </c>
+      <c r="C192">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>78</v>
+      </c>
+      <c r="B193" t="s">
+        <v>45</v>
+      </c>
+      <c r="C193">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>78</v>
+      </c>
+      <c r="B194" t="s">
+        <v>46</v>
+      </c>
+      <c r="C194">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>78</v>
+      </c>
+      <c r="B195" t="s">
+        <v>47</v>
+      </c>
+      <c r="C195">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>78</v>
+      </c>
+      <c r="B196" t="s">
+        <v>48</v>
+      </c>
+      <c r="C196">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
         <v>79</v>
       </c>
-      <c r="B77" t="s">
-        <v>41</v>
-      </c>
-      <c r="C77">
-        <v>5.418069230769231E-9</v>
+      <c r="B197" t="s">
+        <v>41</v>
+      </c>
+      <c r="C197">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>79</v>
+      </c>
+      <c r="B198" t="s">
+        <v>45</v>
+      </c>
+      <c r="C198">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>79</v>
+      </c>
+      <c r="B199" t="s">
+        <v>46</v>
+      </c>
+      <c r="C199">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>79</v>
+      </c>
+      <c r="B200" t="s">
+        <v>47</v>
+      </c>
+      <c r="C200">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>79</v>
+      </c>
+      <c r="B201" t="s">
+        <v>48</v>
+      </c>
+      <c r="C201">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>80</v>
+      </c>
+      <c r="B202" t="s">
+        <v>41</v>
+      </c>
+      <c r="C202">
+        <v>4.1953846153846158E-10</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>80</v>
+      </c>
+      <c r="B203" t="s">
+        <v>45</v>
+      </c>
+      <c r="C203">
+        <v>4.1953846153846158E-10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>80</v>
+      </c>
+      <c r="B204" t="s">
+        <v>46</v>
+      </c>
+      <c r="C204">
+        <v>4.1953846153846158E-10</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>80</v>
+      </c>
+      <c r="B205" t="s">
+        <v>47</v>
+      </c>
+      <c r="C205">
+        <v>4.1953846153846158E-10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>80</v>
+      </c>
+      <c r="B206" t="s">
+        <v>48</v>
+      </c>
+      <c r="C206">
+        <v>4.1953846153846158E-10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>81</v>
+      </c>
+      <c r="B207" t="s">
+        <v>41</v>
+      </c>
+      <c r="C207">
+        <v>1.526538461538462E-9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>81</v>
+      </c>
+      <c r="B208" t="s">
+        <v>45</v>
+      </c>
+      <c r="C208">
+        <v>1.526538461538462E-9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>81</v>
+      </c>
+      <c r="B209" t="s">
+        <v>46</v>
+      </c>
+      <c r="C209">
+        <v>1.526538461538462E-9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>81</v>
+      </c>
+      <c r="B210" t="s">
+        <v>47</v>
+      </c>
+      <c r="C210">
+        <v>1.526538461538462E-9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>81</v>
+      </c>
+      <c r="B211" t="s">
+        <v>48</v>
+      </c>
+      <c r="C211">
+        <v>1.526538461538462E-9</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>82</v>
+      </c>
+      <c r="B212" t="s">
+        <v>41</v>
+      </c>
+      <c r="C212">
+        <v>1.1111538461538459E-9</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>82</v>
+      </c>
+      <c r="B213" t="s">
+        <v>45</v>
+      </c>
+      <c r="C213">
+        <v>1.1111538461538459E-9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>82</v>
+      </c>
+      <c r="B214" t="s">
+        <v>46</v>
+      </c>
+      <c r="C214">
+        <v>1.1111538461538459E-9</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>82</v>
+      </c>
+      <c r="B215" t="s">
+        <v>47</v>
+      </c>
+      <c r="C215">
+        <v>1.1111538461538459E-9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>82</v>
+      </c>
+      <c r="B216" t="s">
+        <v>48</v>
+      </c>
+      <c r="C216">
+        <v>1.1111538461538459E-9</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>83</v>
+      </c>
+      <c r="B217" t="s">
+        <v>41</v>
+      </c>
+      <c r="C217">
+        <v>2.886923076923077E-9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>83</v>
+      </c>
+      <c r="B218" t="s">
+        <v>45</v>
+      </c>
+      <c r="C218">
+        <v>2.886923076923077E-9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>83</v>
+      </c>
+      <c r="B219" t="s">
+        <v>46</v>
+      </c>
+      <c r="C219">
+        <v>2.886923076923077E-9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>83</v>
+      </c>
+      <c r="B220" t="s">
+        <v>47</v>
+      </c>
+      <c r="C220">
+        <v>2.886923076923077E-9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>83</v>
+      </c>
+      <c r="B221" t="s">
+        <v>48</v>
+      </c>
+      <c r="C221">
+        <v>2.886923076923077E-9</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>84</v>
+      </c>
+      <c r="B222" t="s">
+        <v>41</v>
+      </c>
+      <c r="C222">
+        <v>3.7176923076923079E-9</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>84</v>
+      </c>
+      <c r="B223" t="s">
+        <v>45</v>
+      </c>
+      <c r="C223">
+        <v>3.7176923076923079E-9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>84</v>
+      </c>
+      <c r="B224" t="s">
+        <v>46</v>
+      </c>
+      <c r="C224">
+        <v>3.7176923076923079E-9</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>84</v>
+      </c>
+      <c r="B225" t="s">
+        <v>47</v>
+      </c>
+      <c r="C225">
+        <v>3.7176923076923079E-9</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>84</v>
+      </c>
+      <c r="B226" t="s">
+        <v>48</v>
+      </c>
+      <c r="C226">
+        <v>3.7176923076923079E-9</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>85</v>
+      </c>
+      <c r="B227" t="s">
+        <v>41</v>
+      </c>
+      <c r="C227">
+        <v>5.4207692307692314E-9</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>85</v>
+      </c>
+      <c r="B228" t="s">
+        <v>45</v>
+      </c>
+      <c r="C228">
+        <v>5.4207692307692314E-9</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>85</v>
+      </c>
+      <c r="B229" t="s">
+        <v>46</v>
+      </c>
+      <c r="C229">
+        <v>5.4207692307692314E-9</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>85</v>
+      </c>
+      <c r="B230" t="s">
+        <v>47</v>
+      </c>
+      <c r="C230">
+        <v>5.4207692307692314E-9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>85</v>
+      </c>
+      <c r="B231" t="s">
+        <v>48</v>
+      </c>
+      <c r="C231">
+        <v>5.4207692307692314E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace single colon with double colon
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC4FBFB-BDAB-4FCF-BA34-EB1D77D18328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6A0B20-A826-44E7-96D9-E1BB1D5468E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,24 +162,9 @@
     <t>Carbon dioxide, fossil</t>
   </si>
   <si>
-    <t>air:low population density, long-term</t>
-  </si>
-  <si>
-    <t>air:lower stratosphere + upper troposphere</t>
-  </si>
-  <si>
-    <t>air:non-urban air or from high stacks</t>
-  </si>
-  <si>
-    <t>air:urban air close to ground</t>
-  </si>
-  <si>
     <t>Carbon dioxide, from soil or biomass stock</t>
   </si>
   <si>
-    <t>air:indoor</t>
-  </si>
-  <si>
     <t>Dinitrogen monoxide</t>
   </si>
   <si>
@@ -283,6 +268,21 @@
   </si>
   <si>
     <t>Sulfur hexafluoride</t>
+  </si>
+  <si>
+    <t>air::low population density, long-term</t>
+  </si>
+  <si>
+    <t>air::lower stratosphere + upper troposphere</t>
+  </si>
+  <si>
+    <t>air::non-urban air or from high stacks</t>
+  </si>
+  <si>
+    <t>air::urban air close to ground</t>
+  </si>
+  <si>
+    <t>air::indoor</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,7 @@
   <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,7 +1056,7 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C40">
         <v>2.076923076923077E-13</v>
@@ -1067,7 +1067,7 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C41">
         <v>2.076923076923077E-13</v>
@@ -1078,7 +1078,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <v>2.076923076923077E-13</v>
@@ -1089,7 +1089,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>2.076923076923077E-13</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="C45">
         <v>2.076923076923077E-13</v>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C46">
         <v>2.076923076923077E-13</v>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C47">
         <v>2.076923076923077E-13</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C48">
         <v>2.076923076923077E-13</v>
@@ -1152,10 +1152,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C49">
         <v>2.076923076923077E-13</v>
@@ -1177,7 +1177,7 @@
         <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C51">
         <v>4.1538461538461543E-12</v>
@@ -1188,7 +1188,7 @@
         <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C52">
         <v>4.1538461538461543E-12</v>
@@ -1199,7 +1199,7 @@
         <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C53">
         <v>4.1538461538461543E-12</v>
@@ -1210,7 +1210,7 @@
         <v>40</v>
       </c>
       <c r="B54" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C54">
         <v>4.1538461538461543E-12</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
         <v>41</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C56">
         <v>6.1892307692307702E-11</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C57">
         <v>6.1892307692307702E-11</v>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C58">
         <v>6.1892307692307702E-11</v>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C59">
         <v>6.1892307692307702E-11</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C61">
         <v>3.2192307692307691E-10</v>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C62">
         <v>3.2192307692307691E-10</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C63">
         <v>3.2192307692307691E-10</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C64">
         <v>3.2192307692307691E-10</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
         <v>41</v>
@@ -1339,10 +1339,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C66">
         <v>4.0084615384615378E-11</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C67">
         <v>4.0084615384615378E-11</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C68">
         <v>4.0084615384615378E-11</v>
@@ -1372,10 +1372,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C69">
         <v>4.0084615384615378E-11</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B70" t="s">
         <v>41</v>
@@ -1394,10 +1394,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C71">
         <v>1.1443846153846149E-9</v>
@@ -1405,10 +1405,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C72">
         <v>1.1443846153846149E-9</v>
@@ -1416,10 +1416,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C73">
         <v>1.1443846153846149E-9</v>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C74">
         <v>1.1443846153846149E-9</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B75" t="s">
         <v>41</v>
@@ -1449,10 +1449,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C76">
         <v>1.3686923076923081E-9</v>
@@ -1460,10 +1460,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B77" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C77">
         <v>1.3686923076923081E-9</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C78">
         <v>1.3686923076923081E-9</v>
@@ -1482,10 +1482,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B79" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C79">
         <v>1.3686923076923081E-9</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B80" t="s">
         <v>41</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B81" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C81">
         <v>1.9481538461538459E-10</v>
@@ -1515,10 +1515,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B82" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C82">
         <v>1.9481538461538459E-10</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B83" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C83">
         <v>1.9481538461538459E-10</v>
@@ -1537,10 +1537,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B84" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C84">
         <v>1.9481538461538459E-10</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B85" t="s">
         <v>41</v>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B86" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C86">
         <v>3.4684615384615383E-11</v>
@@ -1570,10 +1570,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B87" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C87">
         <v>3.4684615384615383E-11</v>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B88" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C88">
         <v>3.4684615384615383E-11</v>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C89">
         <v>3.4684615384615383E-11</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B90" t="s">
         <v>41</v>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B91" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C91">
         <v>2.076923076923077E-13</v>
@@ -1625,10 +1625,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C92">
         <v>2.076923076923077E-13</v>
@@ -1636,10 +1636,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B93" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C93">
         <v>2.076923076923077E-13</v>
@@ -1647,10 +1647,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C94">
         <v>2.076923076923077E-13</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B95" t="s">
         <v>41</v>
@@ -1669,10 +1669,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B96" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C96">
         <v>1.9979999999999999E-9</v>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B97" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C97">
         <v>1.9979999999999999E-9</v>
@@ -1691,10 +1691,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B98" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C98">
         <v>1.9979999999999999E-9</v>
@@ -1702,10 +1702,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B99" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C99">
         <v>1.9979999999999999E-9</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B100" t="s">
         <v>41</v>
@@ -1724,10 +1724,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B101" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C101">
         <v>4.8807692307692314E-10</v>
@@ -1735,10 +1735,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B102" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C102">
         <v>4.8807692307692314E-10</v>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B103" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C103">
         <v>4.8807692307692314E-10</v>
@@ -1757,10 +1757,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B104" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C104">
         <v>4.8807692307692314E-10</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B105" t="s">
         <v>41</v>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B106" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C106">
         <v>1.9938461538461541E-11</v>
@@ -1790,10 +1790,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C107">
         <v>1.9938461538461541E-11</v>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B108" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C108">
         <v>1.9938461538461541E-11</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B109" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C109">
         <v>1.9938461538461541E-11</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
@@ -1834,10 +1834,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C111">
         <v>1.3188461538461541E-10</v>
@@ -1845,10 +1845,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B112" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C112">
         <v>1.3188461538461541E-10</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C113">
         <v>1.3188461538461541E-10</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C114">
         <v>1.3188461538461541E-10</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B115" t="s">
         <v>41</v>
@@ -1889,10 +1889,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B116" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C116">
         <v>1.7695384615384611E-9</v>
@@ -1900,10 +1900,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B117" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C117">
         <v>1.7695384615384611E-9</v>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B118" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C118">
         <v>1.7695384615384611E-9</v>
@@ -1922,10 +1922,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B119" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C119">
         <v>1.7695384615384611E-9</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B120" t="s">
         <v>41</v>
@@ -1944,10 +1944,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B121" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C121">
         <v>2.554615384615385E-9</v>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B122" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C122">
         <v>2.554615384615385E-9</v>
@@ -1966,10 +1966,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B123" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C123">
         <v>2.554615384615385E-9</v>
@@ -1977,10 +1977,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B124" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C124">
         <v>2.554615384615385E-9</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B125" t="s">
         <v>41</v>
@@ -1999,10 +1999,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B126" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C126">
         <v>7.6638461538461539E-10</v>
@@ -2010,10 +2010,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B127" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C127">
         <v>7.6638461538461539E-10</v>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B128" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C128">
         <v>7.6638461538461539E-10</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B129" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C129">
         <v>7.6638461538461539E-10</v>
@@ -2057,7 +2057,7 @@
         <v>42</v>
       </c>
       <c r="B131" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C131">
         <v>2.8661538461538461E-12</v>
@@ -2068,7 +2068,7 @@
         <v>42</v>
       </c>
       <c r="B132" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C132">
         <v>2.8661538461538461E-12</v>
@@ -2079,7 +2079,7 @@
         <v>42</v>
       </c>
       <c r="B133" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C133">
         <v>2.8661538461538461E-12</v>
@@ -2090,7 +2090,7 @@
         <v>42</v>
       </c>
       <c r="B134" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C134">
         <v>2.8661538461538461E-12</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B135" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C135">
         <v>7.0615384615384616E-12</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B136" t="s">
         <v>41</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B137" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C137">
         <v>6.2307692307692306E-13</v>
@@ -2131,10 +2131,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B138" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C138">
         <v>6.2307692307692306E-13</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B139" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C139">
         <v>6.2307692307692306E-13</v>
@@ -2153,10 +2153,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B140" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C140">
         <v>6.2307692307692306E-13</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B141" t="s">
         <v>41</v>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B142" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C142">
         <v>4.29923076923077E-10</v>
@@ -2186,10 +2186,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B143" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C143">
         <v>4.29923076923077E-10</v>
@@ -2197,10 +2197,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B144" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C144">
         <v>4.29923076923077E-10</v>
@@ -2208,10 +2208,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B145" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C145">
         <v>4.29923076923077E-10</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B146" t="s">
         <v>41</v>
@@ -2230,10 +2230,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B147" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C147">
         <v>1.4849999999999999E-9</v>
@@ -2241,10 +2241,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B148" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C148">
         <v>1.4849999999999999E-9</v>
@@ -2252,10 +2252,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B149" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C149">
         <v>1.4849999999999999E-9</v>
@@ -2263,10 +2263,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B150" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C150">
         <v>1.4849999999999999E-9</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B151" t="s">
         <v>41</v>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B152" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C152">
         <v>4.3823076923076919E-10</v>
@@ -2296,10 +2296,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B153" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C153">
         <v>4.3823076923076919E-10</v>
@@ -2307,10 +2307,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B154" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C154">
         <v>4.3823076923076919E-10</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B155" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C155">
         <v>4.3823076923076919E-10</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B156" t="s">
         <v>41</v>
@@ -2340,10 +2340,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B157" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C157">
         <v>3.2192307692307689E-9</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B158" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C158">
         <v>3.2192307692307689E-9</v>
@@ -2362,10 +2362,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B159" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C159">
         <v>3.2192307692307689E-9</v>
@@ -2373,10 +2373,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B160" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C160">
         <v>3.2192307692307689E-9</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B161" t="s">
         <v>41</v>
@@ -2395,10 +2395,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B162" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C162">
         <v>2.2846153846153851E-12</v>
@@ -2406,10 +2406,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B163" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C163">
         <v>2.2846153846153851E-12</v>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B164" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C164">
         <v>2.2846153846153851E-12</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B165" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C165">
         <v>2.2846153846153851E-12</v>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B166" t="s">
         <v>41</v>
@@ -2450,10 +2450,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B167" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C167">
         <v>2.388461538461538E-9</v>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B168" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C168">
         <v>2.388461538461538E-9</v>
@@ -2472,10 +2472,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B169" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C169">
         <v>2.388461538461538E-9</v>
@@ -2483,10 +2483,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B170" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C170">
         <v>2.388461538461538E-9</v>
@@ -2494,7 +2494,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B171" t="s">
         <v>41</v>
@@ -2505,10 +2505,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B172" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C172">
         <v>3.7176923076923081E-11</v>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B173" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C173">
         <v>3.7176923076923081E-11</v>
@@ -2527,10 +2527,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B174" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C174">
         <v>3.7176923076923081E-11</v>
@@ -2538,10 +2538,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B175" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C175">
         <v>3.7176923076923081E-11</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B176" t="s">
         <v>41</v>
@@ -2560,10 +2560,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B177" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C177">
         <v>1.6968461538461539E-10</v>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B178" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C178">
         <v>1.6968461538461539E-10</v>
@@ -2582,10 +2582,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B179" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C179">
         <v>1.6968461538461539E-10</v>
@@ -2593,10 +2593,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B180" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C180">
         <v>1.6968461538461539E-10</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B181" t="s">
         <v>41</v>
@@ -2615,10 +2615,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B182" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C182">
         <v>7.4769230769230768E-12</v>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B183" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C183">
         <v>7.4769230769230768E-12</v>
@@ -2637,10 +2637,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B184" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C184">
         <v>7.4769230769230768E-12</v>
@@ -2648,10 +2648,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B185" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C185">
         <v>7.4769230769230768E-12</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B186" t="s">
         <v>41</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B187" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="C187">
         <v>7.0615384615384616E-12</v>
@@ -2681,10 +2681,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B188" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C188">
         <v>7.0615384615384616E-12</v>
@@ -2692,10 +2692,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B189" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C189">
         <v>7.0615384615384616E-12</v>
@@ -2703,10 +2703,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B190" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C190">
         <v>7.0615384615384616E-12</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B191" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C191">
         <v>7.0615384615384616E-12</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B192" t="s">
         <v>41</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B193" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C193">
         <v>3.1153846153846161E-12</v>
@@ -2747,10 +2747,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B194" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C194">
         <v>3.1153846153846161E-12</v>
@@ -2758,10 +2758,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B195" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C195">
         <v>3.1153846153846161E-12</v>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B196" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C196">
         <v>3.1153846153846161E-12</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B197" t="s">
         <v>41</v>
@@ -2791,10 +2791,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B198" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C198">
         <v>7.0615384615384616E-12</v>
@@ -2802,10 +2802,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B199" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C199">
         <v>7.0615384615384616E-12</v>
@@ -2813,10 +2813,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B200" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C200">
         <v>7.0615384615384616E-12</v>
@@ -2824,10 +2824,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B201" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C201">
         <v>7.0615384615384616E-12</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B202" t="s">
         <v>41</v>
@@ -2846,10 +2846,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B203" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C203">
         <v>4.1953846153846158E-10</v>
@@ -2857,10 +2857,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B204" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C204">
         <v>4.1953846153846158E-10</v>
@@ -2868,10 +2868,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B205" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C205">
         <v>4.1953846153846158E-10</v>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B206" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C206">
         <v>4.1953846153846158E-10</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B207" t="s">
         <v>41</v>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B208" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C208">
         <v>1.526538461538462E-9</v>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B209" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C209">
         <v>1.526538461538462E-9</v>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B210" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C210">
         <v>1.526538461538462E-9</v>
@@ -2934,10 +2934,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B211" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C211">
         <v>1.526538461538462E-9</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B212" t="s">
         <v>41</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B213" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C213">
         <v>1.1111538461538459E-9</v>
@@ -2967,10 +2967,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B214" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C214">
         <v>1.1111538461538459E-9</v>
@@ -2978,10 +2978,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B215" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C215">
         <v>1.1111538461538459E-9</v>
@@ -2989,10 +2989,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B216" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C216">
         <v>1.1111538461538459E-9</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B217" t="s">
         <v>41</v>
@@ -3011,10 +3011,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B218" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C218">
         <v>2.886923076923077E-9</v>
@@ -3022,10 +3022,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B219" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C219">
         <v>2.886923076923077E-9</v>
@@ -3033,10 +3033,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B220" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C220">
         <v>2.886923076923077E-9</v>
@@ -3044,10 +3044,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B221" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C221">
         <v>2.886923076923077E-9</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B222" t="s">
         <v>41</v>
@@ -3066,10 +3066,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B223" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C223">
         <v>3.7176923076923079E-9</v>
@@ -3077,10 +3077,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B224" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C224">
         <v>3.7176923076923079E-9</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B225" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C225">
         <v>3.7176923076923079E-9</v>
@@ -3099,10 +3099,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B226" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C226">
         <v>3.7176923076923079E-9</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B227" t="s">
         <v>41</v>
@@ -3121,10 +3121,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B228" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C228">
         <v>5.4207692307692314E-9</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B229" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C229">
         <v>5.4207692307692314E-9</v>
@@ -3143,10 +3143,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B230" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C230">
         <v>5.4207692307692314E-9</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B231" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C231">
         <v>5.4207692307692314E-9</v>

</xml_diff>

<commit_message>
Add strategies to generate "subcategories" for CBI method
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904404BE-FB7F-412E-9C87-0C9FABB7F5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223F0831-DB65-40B5-BA39-F73BA16A1B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -274,6 +274,27 @@
   </si>
   <si>
     <t>air::urban air close to ground</t>
+  </si>
+  <si>
+    <t>air::low population density, long-term</t>
+  </si>
+  <si>
+    <t>air::lower stratosphere + upper troposphere</t>
+  </si>
+  <si>
+    <t>air::non-urban air or from high stacks</t>
+  </si>
+  <si>
+    <t>air::indoor</t>
+  </si>
+  <si>
+    <t>soil::agricultural</t>
+  </si>
+  <si>
+    <t>soil::forestry</t>
+  </si>
+  <si>
+    <t>soil::industrial</t>
   </si>
 </sst>
 </file>
@@ -600,16 +621,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1044,419 +1065,2058 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C40">
-        <v>2.8661538461538461E-12</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C41">
-        <v>2.076923076923077E-13</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C42">
-        <v>2.076923076923077E-13</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C43">
-        <v>-2.076923076923077E-13</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
       </c>
       <c r="C44">
-        <v>6.1892307692307702E-11</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C45">
-        <v>3.2171538461538461E-10</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C46">
-        <v>1.143969230769231E-9</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C47">
-        <v>1.3678615384615381E-9</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C48">
-        <v>1.9481538461538459E-10</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
         <v>41</v>
       </c>
       <c r="C49">
-        <v>3.4684615384615383E-11</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C50">
-        <v>1.9969615384615379E-9</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C51">
-        <v>4.8703846153846161E-10</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C52">
-        <v>1.9938461538461541E-11</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C53">
-        <v>1.3188461538461541E-10</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B54" t="s">
         <v>41</v>
       </c>
       <c r="C54">
-        <v>1.7687076923076921E-9</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C55">
-        <v>2.5629230769230769E-9</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C56">
-        <v>7.6659230769230773E-10</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C57">
-        <v>7.4769230769230768E-12</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C58">
-        <v>6.2307692307692306E-13</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C59">
-        <v>4.29923076923077E-10</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C60">
-        <v>1.4858307692307699E-9</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="C61">
-        <v>4.3740000000000001E-10</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C62">
-        <v>3.2090538461538469E-9</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C63">
-        <v>2.2846153846153851E-12</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
       </c>
       <c r="C64">
-        <v>2.3982230769230768E-9</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C65">
-        <v>3.7176923076923081E-11</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C66">
-        <v>1.6968461538461539E-10</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C67">
-        <v>7.4769230769230768E-12</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C68">
-        <v>7.0615384615384616E-12</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
         <v>41</v>
       </c>
       <c r="C69">
-        <v>3.1153846153846161E-12</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C70">
-        <v>7.0615384615384616E-12</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C71">
-        <v>4.1933076923076919E-10</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C72">
-        <v>1.5263307692307689E-9</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C73">
-        <v>1.111569230769231E-9</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B74" t="s">
         <v>41</v>
       </c>
       <c r="C74">
-        <v>2.8777846153846162E-9</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C75">
-        <v>3.714576923076923E-9</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C76">
-        <v>1.969753846153846E-9</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77">
+        <v>1.143969230769231E-9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>49</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78">
+        <v>1.143969230769231E-9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79">
+        <v>1.3678615384615381E-9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>50</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80">
+        <v>1.3678615384615381E-9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
+        <v>1.3678615384615381E-9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82">
+        <v>1.3678615384615381E-9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <v>1.3678615384615381E-9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>51</v>
+      </c>
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>51</v>
+      </c>
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>51</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+      <c r="C86">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>51</v>
+      </c>
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+      <c r="C87">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>51</v>
+      </c>
+      <c r="B88" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88">
+        <v>1.9481538461538459E-10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>52</v>
+      </c>
+      <c r="B89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" t="s">
+        <v>84</v>
+      </c>
+      <c r="C91">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" t="s">
+        <v>85</v>
+      </c>
+      <c r="C92">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>52</v>
+      </c>
+      <c r="B93" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93">
+        <v>3.4684615384615383E-11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>53</v>
+      </c>
+      <c r="B94" t="s">
+        <v>41</v>
+      </c>
+      <c r="C94">
+        <v>1.9969615384615379E-9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95" t="s">
+        <v>83</v>
+      </c>
+      <c r="C95">
+        <v>1.9969615384615379E-9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>53</v>
+      </c>
+      <c r="B96" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96">
+        <v>1.9969615384615379E-9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>53</v>
+      </c>
+      <c r="B97" t="s">
+        <v>85</v>
+      </c>
+      <c r="C97">
+        <v>1.9969615384615379E-9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98">
+        <v>1.9969615384615379E-9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>54</v>
+      </c>
+      <c r="B99" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99">
+        <v>4.8703846153846161E-10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>54</v>
+      </c>
+      <c r="B100" t="s">
+        <v>83</v>
+      </c>
+      <c r="C100">
+        <v>4.8703846153846161E-10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101" t="s">
+        <v>84</v>
+      </c>
+      <c r="C101">
+        <v>4.8703846153846161E-10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>54</v>
+      </c>
+      <c r="B102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C102">
+        <v>4.8703846153846161E-10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>54</v>
+      </c>
+      <c r="B103" t="s">
+        <v>82</v>
+      </c>
+      <c r="C103">
+        <v>4.8703846153846161E-10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105" t="s">
+        <v>83</v>
+      </c>
+      <c r="C105">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>55</v>
+      </c>
+      <c r="B106" t="s">
+        <v>84</v>
+      </c>
+      <c r="C106">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>55</v>
+      </c>
+      <c r="B107" t="s">
+        <v>85</v>
+      </c>
+      <c r="C107">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>55</v>
+      </c>
+      <c r="B108" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108">
+        <v>1.9938461538461541E-11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>56</v>
+      </c>
+      <c r="B109" t="s">
+        <v>41</v>
+      </c>
+      <c r="C109">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>56</v>
+      </c>
+      <c r="B110" t="s">
+        <v>83</v>
+      </c>
+      <c r="C110">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>56</v>
+      </c>
+      <c r="B111" t="s">
+        <v>84</v>
+      </c>
+      <c r="C111">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>56</v>
+      </c>
+      <c r="B112" t="s">
+        <v>85</v>
+      </c>
+      <c r="C112">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>56</v>
+      </c>
+      <c r="B113" t="s">
+        <v>82</v>
+      </c>
+      <c r="C113">
+        <v>1.3188461538461541E-10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>57</v>
+      </c>
+      <c r="B114" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114">
+        <v>1.7687076923076921E-9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>57</v>
+      </c>
+      <c r="B115" t="s">
+        <v>83</v>
+      </c>
+      <c r="C115">
+        <v>1.7687076923076921E-9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>57</v>
+      </c>
+      <c r="B116" t="s">
+        <v>84</v>
+      </c>
+      <c r="C116">
+        <v>1.7687076923076921E-9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>57</v>
+      </c>
+      <c r="B117" t="s">
+        <v>85</v>
+      </c>
+      <c r="C117">
+        <v>1.7687076923076921E-9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>57</v>
+      </c>
+      <c r="B118" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118">
+        <v>1.7687076923076921E-9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>58</v>
+      </c>
+      <c r="B119" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119">
+        <v>2.5629230769230769E-9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>58</v>
+      </c>
+      <c r="B120" t="s">
+        <v>83</v>
+      </c>
+      <c r="C120">
+        <v>2.5629230769230769E-9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>58</v>
+      </c>
+      <c r="B121" t="s">
+        <v>84</v>
+      </c>
+      <c r="C121">
+        <v>2.5629230769230769E-9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>58</v>
+      </c>
+      <c r="B122" t="s">
+        <v>85</v>
+      </c>
+      <c r="C122">
+        <v>2.5629230769230769E-9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>58</v>
+      </c>
+      <c r="B123" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123">
+        <v>2.5629230769230769E-9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>59</v>
+      </c>
+      <c r="B124" t="s">
+        <v>41</v>
+      </c>
+      <c r="C124">
+        <v>7.6659230769230773E-10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>59</v>
+      </c>
+      <c r="B125" t="s">
+        <v>83</v>
+      </c>
+      <c r="C125">
+        <v>7.6659230769230773E-10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>59</v>
+      </c>
+      <c r="B126" t="s">
+        <v>84</v>
+      </c>
+      <c r="C126">
+        <v>7.6659230769230773E-10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>59</v>
+      </c>
+      <c r="B127" t="s">
+        <v>85</v>
+      </c>
+      <c r="C127">
+        <v>7.6659230769230773E-10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>59</v>
+      </c>
+      <c r="B128" t="s">
+        <v>82</v>
+      </c>
+      <c r="C128">
+        <v>7.6659230769230773E-10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>81</v>
+      </c>
+      <c r="B129" t="s">
+        <v>41</v>
+      </c>
+      <c r="C129">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>60</v>
+      </c>
+      <c r="B130" t="s">
+        <v>41</v>
+      </c>
+      <c r="C130">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>60</v>
+      </c>
+      <c r="B131" t="s">
+        <v>83</v>
+      </c>
+      <c r="C131">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>60</v>
+      </c>
+      <c r="B132" t="s">
+        <v>84</v>
+      </c>
+      <c r="C132">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>60</v>
+      </c>
+      <c r="B133" t="s">
+        <v>85</v>
+      </c>
+      <c r="C133">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>60</v>
+      </c>
+      <c r="B134" t="s">
+        <v>82</v>
+      </c>
+      <c r="C134">
+        <v>6.2307692307692306E-13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>61</v>
+      </c>
+      <c r="B135" t="s">
+        <v>41</v>
+      </c>
+      <c r="C135">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>61</v>
+      </c>
+      <c r="B136" t="s">
+        <v>83</v>
+      </c>
+      <c r="C136">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>61</v>
+      </c>
+      <c r="B137" t="s">
+        <v>84</v>
+      </c>
+      <c r="C137">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>61</v>
+      </c>
+      <c r="B138" t="s">
+        <v>85</v>
+      </c>
+      <c r="C138">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>61</v>
+      </c>
+      <c r="B139" t="s">
+        <v>82</v>
+      </c>
+      <c r="C139">
+        <v>4.29923076923077E-10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>62</v>
+      </c>
+      <c r="B140" t="s">
+        <v>41</v>
+      </c>
+      <c r="C140">
+        <v>1.4858307692307699E-9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>62</v>
+      </c>
+      <c r="B141" t="s">
+        <v>83</v>
+      </c>
+      <c r="C141">
+        <v>1.4858307692307699E-9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>62</v>
+      </c>
+      <c r="B142" t="s">
+        <v>84</v>
+      </c>
+      <c r="C142">
+        <v>1.4858307692307699E-9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>62</v>
+      </c>
+      <c r="B143" t="s">
+        <v>85</v>
+      </c>
+      <c r="C143">
+        <v>1.4858307692307699E-9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>62</v>
+      </c>
+      <c r="B144" t="s">
+        <v>82</v>
+      </c>
+      <c r="C144">
+        <v>1.4858307692307699E-9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>63</v>
+      </c>
+      <c r="B145" t="s">
+        <v>41</v>
+      </c>
+      <c r="C145">
+        <v>4.3740000000000001E-10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>63</v>
+      </c>
+      <c r="B146" t="s">
+        <v>83</v>
+      </c>
+      <c r="C146">
+        <v>4.3740000000000001E-10</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>63</v>
+      </c>
+      <c r="B147" t="s">
+        <v>84</v>
+      </c>
+      <c r="C147">
+        <v>4.3740000000000001E-10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>63</v>
+      </c>
+      <c r="B148" t="s">
+        <v>85</v>
+      </c>
+      <c r="C148">
+        <v>4.3740000000000001E-10</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>63</v>
+      </c>
+      <c r="B149" t="s">
+        <v>82</v>
+      </c>
+      <c r="C149">
+        <v>4.3740000000000001E-10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>64</v>
+      </c>
+      <c r="B150" t="s">
+        <v>41</v>
+      </c>
+      <c r="C150">
+        <v>3.2090538461538469E-9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>64</v>
+      </c>
+      <c r="B151" t="s">
+        <v>83</v>
+      </c>
+      <c r="C151">
+        <v>3.2090538461538469E-9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>64</v>
+      </c>
+      <c r="B152" t="s">
+        <v>84</v>
+      </c>
+      <c r="C152">
+        <v>3.2090538461538469E-9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>64</v>
+      </c>
+      <c r="B153" t="s">
+        <v>85</v>
+      </c>
+      <c r="C153">
+        <v>3.2090538461538469E-9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>64</v>
+      </c>
+      <c r="B154" t="s">
+        <v>82</v>
+      </c>
+      <c r="C154">
+        <v>3.2090538461538469E-9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>65</v>
+      </c>
+      <c r="B155" t="s">
+        <v>41</v>
+      </c>
+      <c r="C155">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>65</v>
+      </c>
+      <c r="B156" t="s">
+        <v>83</v>
+      </c>
+      <c r="C156">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>65</v>
+      </c>
+      <c r="B157" t="s">
+        <v>84</v>
+      </c>
+      <c r="C157">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>65</v>
+      </c>
+      <c r="B158" t="s">
+        <v>85</v>
+      </c>
+      <c r="C158">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>65</v>
+      </c>
+      <c r="B159" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159">
+        <v>2.2846153846153851E-12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>66</v>
+      </c>
+      <c r="B160" t="s">
+        <v>41</v>
+      </c>
+      <c r="C160">
+        <v>2.3982230769230768E-9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>66</v>
+      </c>
+      <c r="B161" t="s">
+        <v>83</v>
+      </c>
+      <c r="C161">
+        <v>2.3982230769230768E-9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>66</v>
+      </c>
+      <c r="B162" t="s">
+        <v>84</v>
+      </c>
+      <c r="C162">
+        <v>2.3982230769230768E-9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>66</v>
+      </c>
+      <c r="B163" t="s">
+        <v>85</v>
+      </c>
+      <c r="C163">
+        <v>2.3982230769230768E-9</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>66</v>
+      </c>
+      <c r="B164" t="s">
+        <v>82</v>
+      </c>
+      <c r="C164">
+        <v>2.3982230769230768E-9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>67</v>
+      </c>
+      <c r="B165" t="s">
+        <v>41</v>
+      </c>
+      <c r="C165">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>67</v>
+      </c>
+      <c r="B166" t="s">
+        <v>83</v>
+      </c>
+      <c r="C166">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>67</v>
+      </c>
+      <c r="B167" t="s">
+        <v>84</v>
+      </c>
+      <c r="C167">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>67</v>
+      </c>
+      <c r="B168" t="s">
+        <v>85</v>
+      </c>
+      <c r="C168">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>67</v>
+      </c>
+      <c r="B169" t="s">
+        <v>82</v>
+      </c>
+      <c r="C169">
+        <v>3.7176923076923081E-11</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>68</v>
+      </c>
+      <c r="B170" t="s">
+        <v>41</v>
+      </c>
+      <c r="C170">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>68</v>
+      </c>
+      <c r="B171" t="s">
+        <v>83</v>
+      </c>
+      <c r="C171">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>68</v>
+      </c>
+      <c r="B172" t="s">
+        <v>84</v>
+      </c>
+      <c r="C172">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>68</v>
+      </c>
+      <c r="B173" t="s">
+        <v>85</v>
+      </c>
+      <c r="C173">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>68</v>
+      </c>
+      <c r="B174" t="s">
+        <v>82</v>
+      </c>
+      <c r="C174">
+        <v>1.6968461538461539E-10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>69</v>
+      </c>
+      <c r="B175" t="s">
+        <v>41</v>
+      </c>
+      <c r="C175">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>69</v>
+      </c>
+      <c r="B176" t="s">
+        <v>83</v>
+      </c>
+      <c r="C176">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>69</v>
+      </c>
+      <c r="B177" t="s">
+        <v>84</v>
+      </c>
+      <c r="C177">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>69</v>
+      </c>
+      <c r="B178" t="s">
+        <v>85</v>
+      </c>
+      <c r="C178">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>69</v>
+      </c>
+      <c r="B179" t="s">
+        <v>82</v>
+      </c>
+      <c r="C179">
+        <v>7.4769230769230768E-12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>70</v>
+      </c>
+      <c r="B180" t="s">
+        <v>41</v>
+      </c>
+      <c r="C180">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>70</v>
+      </c>
+      <c r="B181" t="s">
+        <v>83</v>
+      </c>
+      <c r="C181">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>70</v>
+      </c>
+      <c r="B182" t="s">
+        <v>84</v>
+      </c>
+      <c r="C182">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>70</v>
+      </c>
+      <c r="B183" t="s">
+        <v>85</v>
+      </c>
+      <c r="C183">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>70</v>
+      </c>
+      <c r="B184" t="s">
+        <v>82</v>
+      </c>
+      <c r="C184">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>70</v>
+      </c>
+      <c r="B185" t="s">
+        <v>86</v>
+      </c>
+      <c r="C185">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>71</v>
+      </c>
+      <c r="B186" t="s">
+        <v>41</v>
+      </c>
+      <c r="C186">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>71</v>
+      </c>
+      <c r="B187" t="s">
+        <v>83</v>
+      </c>
+      <c r="C187">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>71</v>
+      </c>
+      <c r="B188" t="s">
+        <v>84</v>
+      </c>
+      <c r="C188">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>71</v>
+      </c>
+      <c r="B189" t="s">
+        <v>85</v>
+      </c>
+      <c r="C189">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>71</v>
+      </c>
+      <c r="B190" t="s">
+        <v>82</v>
+      </c>
+      <c r="C190">
+        <v>3.1153846153846161E-12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>72</v>
+      </c>
+      <c r="B191" t="s">
+        <v>41</v>
+      </c>
+      <c r="C191">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>72</v>
+      </c>
+      <c r="B192" t="s">
+        <v>83</v>
+      </c>
+      <c r="C192">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>72</v>
+      </c>
+      <c r="B193" t="s">
+        <v>84</v>
+      </c>
+      <c r="C193">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>72</v>
+      </c>
+      <c r="B194" t="s">
+        <v>85</v>
+      </c>
+      <c r="C194">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>72</v>
+      </c>
+      <c r="B195" t="s">
+        <v>82</v>
+      </c>
+      <c r="C195">
+        <v>7.0615384615384616E-12</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>73</v>
+      </c>
+      <c r="B196" t="s">
+        <v>41</v>
+      </c>
+      <c r="C196">
+        <v>4.1933076923076919E-10</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>73</v>
+      </c>
+      <c r="B197" t="s">
+        <v>83</v>
+      </c>
+      <c r="C197">
+        <v>4.1933076923076919E-10</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>73</v>
+      </c>
+      <c r="B198" t="s">
+        <v>84</v>
+      </c>
+      <c r="C198">
+        <v>4.1933076923076919E-10</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>73</v>
+      </c>
+      <c r="B199" t="s">
+        <v>85</v>
+      </c>
+      <c r="C199">
+        <v>4.1933076923076919E-10</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>73</v>
+      </c>
+      <c r="B200" t="s">
+        <v>82</v>
+      </c>
+      <c r="C200">
+        <v>4.1933076923076919E-10</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>74</v>
+      </c>
+      <c r="B201" t="s">
+        <v>41</v>
+      </c>
+      <c r="C201">
+        <v>1.5263307692307689E-9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>74</v>
+      </c>
+      <c r="B202" t="s">
+        <v>83</v>
+      </c>
+      <c r="C202">
+        <v>1.5263307692307689E-9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>74</v>
+      </c>
+      <c r="B203" t="s">
+        <v>84</v>
+      </c>
+      <c r="C203">
+        <v>1.5263307692307689E-9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>74</v>
+      </c>
+      <c r="B204" t="s">
+        <v>85</v>
+      </c>
+      <c r="C204">
+        <v>1.5263307692307689E-9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>74</v>
+      </c>
+      <c r="B205" t="s">
+        <v>82</v>
+      </c>
+      <c r="C205">
+        <v>1.5263307692307689E-9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>75</v>
+      </c>
+      <c r="B206" t="s">
+        <v>41</v>
+      </c>
+      <c r="C206">
+        <v>1.111569230769231E-9</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>75</v>
+      </c>
+      <c r="B207" t="s">
+        <v>83</v>
+      </c>
+      <c r="C207">
+        <v>1.111569230769231E-9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>75</v>
+      </c>
+      <c r="B208" t="s">
+        <v>84</v>
+      </c>
+      <c r="C208">
+        <v>1.111569230769231E-9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>75</v>
+      </c>
+      <c r="B209" t="s">
+        <v>85</v>
+      </c>
+      <c r="C209">
+        <v>1.111569230769231E-9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>75</v>
+      </c>
+      <c r="B210" t="s">
+        <v>82</v>
+      </c>
+      <c r="C210">
+        <v>1.111569230769231E-9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>76</v>
+      </c>
+      <c r="B211" t="s">
+        <v>41</v>
+      </c>
+      <c r="C211">
+        <v>2.8777846153846162E-9</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>76</v>
+      </c>
+      <c r="B212" t="s">
+        <v>83</v>
+      </c>
+      <c r="C212">
+        <v>2.8777846153846162E-9</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>76</v>
+      </c>
+      <c r="B213" t="s">
+        <v>84</v>
+      </c>
+      <c r="C213">
+        <v>2.8777846153846162E-9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>76</v>
+      </c>
+      <c r="B214" t="s">
+        <v>85</v>
+      </c>
+      <c r="C214">
+        <v>2.8777846153846162E-9</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>76</v>
+      </c>
+      <c r="B215" t="s">
+        <v>82</v>
+      </c>
+      <c r="C215">
+        <v>2.8777846153846162E-9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>77</v>
+      </c>
+      <c r="B216" t="s">
+        <v>41</v>
+      </c>
+      <c r="C216">
+        <v>3.714576923076923E-9</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>77</v>
+      </c>
+      <c r="B217" t="s">
+        <v>83</v>
+      </c>
+      <c r="C217">
+        <v>3.714576923076923E-9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>77</v>
+      </c>
+      <c r="B218" t="s">
+        <v>84</v>
+      </c>
+      <c r="C218">
+        <v>3.714576923076923E-9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>77</v>
+      </c>
+      <c r="B219" t="s">
+        <v>85</v>
+      </c>
+      <c r="C219">
+        <v>3.714576923076923E-9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>77</v>
+      </c>
+      <c r="B220" t="s">
+        <v>82</v>
+      </c>
+      <c r="C220">
+        <v>3.714576923076923E-9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>78</v>
+      </c>
+      <c r="B221" t="s">
+        <v>41</v>
+      </c>
+      <c r="C221">
+        <v>1.969753846153846E-9</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
         <v>79</v>
       </c>
-      <c r="B77" t="s">
-        <v>41</v>
-      </c>
-      <c r="C77">
+      <c r="B222" t="s">
+        <v>41</v>
+      </c>
+      <c r="C222">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>79</v>
+      </c>
+      <c r="B223" t="s">
+        <v>83</v>
+      </c>
+      <c r="C223">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>79</v>
+      </c>
+      <c r="B224" t="s">
+        <v>84</v>
+      </c>
+      <c r="C224">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>79</v>
+      </c>
+      <c r="B225" t="s">
+        <v>85</v>
+      </c>
+      <c r="C225">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>79</v>
+      </c>
+      <c r="B226" t="s">
+        <v>82</v>
+      </c>
+      <c r="C226">
         <v>5.418069230769231E-9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add strategy `add_subcategory_methane_air` and update list CFs
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223F0831-DB65-40B5-BA39-F73BA16A1B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1512D2-686E-41AC-A6EE-795D37BCBEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2047,7 @@
         <v>81</v>
       </c>
       <c r="B129" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C129">
         <v>7.4769230769230768E-12</v>

</xml_diff>

<commit_message>
Change CF `Occupation, forest, intesive` from 6.15385E-13 to 3.84615E-13
During matching process (simapro vs bw flows), two alternatives in simapro were matched against one flow in bw, that is:
In Simapro:
- Occupation, forest, intensive, normal = 0.5
- Occupation, forest, intensive, short-cycle = 0.8
In bw:
- Occupation, forest, intensive
Initially I selected 0.8 (precautionary principle), but now, to check if this is the reason of differences, I select 0.5.
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,17 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1512D2-686E-41AC-A6EE-795D37BCBEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABEB814-31DB-44CD-90E5-C2262B53F0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -318,12 +328,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -338,9 +354,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,14 +795,14 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14">
-        <v>6.1538461538461536E-13</v>
+      <c r="B14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3.8461538461538462E-13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add CFs to CBI (biological footprint component)
- "Occupation, lakes, artificial" (natural resource::land) = 7.69231E-13
- "Occupation, water courses, artificial" (natural resource::land) = 7.69231E-13
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABEB814-31DB-44CD-90E5-C2262B53F0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC7313-380C-4585-81B9-173E4CE37D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="92">
   <si>
     <t>name</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>soil::industrial</t>
+  </si>
+  <si>
+    <t>Occupation, lakes, artificial</t>
+  </si>
+  <si>
+    <t>Occupation, water courses, artificial</t>
   </si>
 </sst>
 </file>
@@ -638,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,6 +655,7 @@
     <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -795,10 +802,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>80</v>
       </c>
       <c r="C14" s="2">
@@ -982,41 +989,41 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
+      <c r="A31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="2">
+        <v>7.6923076923076923E-13</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32">
-        <v>7.3076923076923074E-13</v>
+      <c r="A32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="2">
+        <v>7.6923076923076923E-13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>80</v>
       </c>
       <c r="C33">
-        <v>7.3076923076923074E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>80</v>
@@ -1027,7 +1034,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>80</v>
@@ -1038,7 +1045,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>80</v>
@@ -1049,7 +1056,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>80</v>
@@ -1060,7 +1067,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>80</v>
@@ -1071,24 +1078,24 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C39">
-        <v>4.1538461538461543E-12</v>
+        <v>7.3076923076923074E-13</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C40">
-        <v>4.1538461538461543E-12</v>
+        <v>7.3076923076923074E-13</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1096,7 +1103,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>4.1538461538461543E-12</v>
@@ -1107,7 +1114,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <v>4.1538461538461543E-12</v>
@@ -1118,7 +1125,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>4.1538461538461543E-12</v>
@@ -1126,24 +1133,24 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C44">
-        <v>2.8661538461538461E-12</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45">
-        <v>2.8661538461538461E-12</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,7 +1158,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>2.8661538461538461E-12</v>
@@ -1162,7 +1169,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47">
         <v>2.8661538461538461E-12</v>
@@ -1173,7 +1180,7 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C48">
         <v>2.8661538461538461E-12</v>
@@ -1181,24 +1188,24 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C49">
-        <v>2.076923076923077E-13</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50">
-        <v>2.076923076923077E-13</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1206,7 +1213,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C51">
         <v>2.076923076923077E-13</v>
@@ -1217,7 +1224,7 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C52">
         <v>2.076923076923077E-13</v>
@@ -1228,7 +1235,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C53">
         <v>2.076923076923077E-13</v>
@@ -1236,10 +1243,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C54">
         <v>2.076923076923077E-13</v>
@@ -1247,10 +1254,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55">
         <v>2.076923076923077E-13</v>
@@ -1261,7 +1268,7 @@
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C56">
         <v>2.076923076923077E-13</v>
@@ -1272,7 +1279,7 @@
         <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C57">
         <v>2.076923076923077E-13</v>
@@ -1283,7 +1290,7 @@
         <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C58">
         <v>2.076923076923077E-13</v>
@@ -1294,7 +1301,7 @@
         <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C59">
         <v>2.076923076923077E-13</v>
@@ -1302,24 +1309,24 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C60">
-        <v>-2.076923076923077E-13</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C61">
-        <v>-2.076923076923077E-13</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1327,7 +1334,7 @@
         <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C62">
         <v>-2.076923076923077E-13</v>
@@ -1338,7 +1345,7 @@
         <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C63">
         <v>-2.076923076923077E-13</v>
@@ -1346,24 +1353,24 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C64">
-        <v>6.1892307692307702E-11</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C65">
-        <v>6.1892307692307702E-11</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1371,7 +1378,7 @@
         <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C66">
         <v>6.1892307692307702E-11</v>
@@ -1382,7 +1389,7 @@
         <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C67">
         <v>6.1892307692307702E-11</v>
@@ -1393,7 +1400,7 @@
         <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C68">
         <v>6.1892307692307702E-11</v>
@@ -1401,24 +1408,24 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C69">
-        <v>3.2171538461538461E-10</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C70">
-        <v>3.2171538461538461E-10</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1426,7 +1433,7 @@
         <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C71">
         <v>3.2171538461538461E-10</v>
@@ -1437,7 +1444,7 @@
         <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72">
         <v>3.2171538461538461E-10</v>
@@ -1448,7 +1455,7 @@
         <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C73">
         <v>3.2171538461538461E-10</v>
@@ -1456,24 +1463,24 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C74">
-        <v>1.143969230769231E-9</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75">
-        <v>1.143969230769231E-9</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1481,7 +1488,7 @@
         <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C76">
         <v>1.143969230769231E-9</v>
@@ -1492,7 +1499,7 @@
         <v>49</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C77">
         <v>1.143969230769231E-9</v>
@@ -1503,7 +1510,7 @@
         <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C78">
         <v>1.143969230769231E-9</v>
@@ -1511,24 +1518,24 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C79">
-        <v>1.3678615384615381E-9</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C80">
-        <v>1.3678615384615381E-9</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1536,7 +1543,7 @@
         <v>50</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C81">
         <v>1.3678615384615381E-9</v>
@@ -1547,7 +1554,7 @@
         <v>50</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C82">
         <v>1.3678615384615381E-9</v>
@@ -1558,7 +1565,7 @@
         <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C83">
         <v>1.3678615384615381E-9</v>
@@ -1566,24 +1573,24 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C84">
-        <v>1.9481538461538459E-10</v>
+        <v>1.3678615384615381E-9</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C85">
-        <v>1.9481538461538459E-10</v>
+        <v>1.3678615384615381E-9</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -1591,7 +1598,7 @@
         <v>51</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C86">
         <v>1.9481538461538459E-10</v>
@@ -1602,7 +1609,7 @@
         <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C87">
         <v>1.9481538461538459E-10</v>
@@ -1613,7 +1620,7 @@
         <v>51</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C88">
         <v>1.9481538461538459E-10</v>
@@ -1621,24 +1628,24 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C89">
-        <v>3.4684615384615383E-11</v>
+        <v>1.9481538461538459E-10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C90">
-        <v>3.4684615384615383E-11</v>
+        <v>1.9481538461538459E-10</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -1646,7 +1653,7 @@
         <v>52</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C91">
         <v>3.4684615384615383E-11</v>
@@ -1657,7 +1664,7 @@
         <v>52</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C92">
         <v>3.4684615384615383E-11</v>
@@ -1668,7 +1675,7 @@
         <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C93">
         <v>3.4684615384615383E-11</v>
@@ -1676,24 +1683,24 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C94">
-        <v>1.9969615384615379E-9</v>
+        <v>3.4684615384615383E-11</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C95">
-        <v>1.9969615384615379E-9</v>
+        <v>3.4684615384615383E-11</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -1701,7 +1708,7 @@
         <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C96">
         <v>1.9969615384615379E-9</v>
@@ -1712,7 +1719,7 @@
         <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C97">
         <v>1.9969615384615379E-9</v>
@@ -1723,7 +1730,7 @@
         <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C98">
         <v>1.9969615384615379E-9</v>
@@ -1731,24 +1738,24 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C99">
-        <v>4.8703846153846161E-10</v>
+        <v>1.9969615384615379E-9</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B100" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C100">
-        <v>4.8703846153846161E-10</v>
+        <v>1.9969615384615379E-9</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1756,7 +1763,7 @@
         <v>54</v>
       </c>
       <c r="B101" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C101">
         <v>4.8703846153846161E-10</v>
@@ -1767,7 +1774,7 @@
         <v>54</v>
       </c>
       <c r="B102" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C102">
         <v>4.8703846153846161E-10</v>
@@ -1778,7 +1785,7 @@
         <v>54</v>
       </c>
       <c r="B103" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C103">
         <v>4.8703846153846161E-10</v>
@@ -1786,24 +1793,24 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C104">
-        <v>1.9938461538461541E-11</v>
+        <v>4.8703846153846161E-10</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B105" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C105">
-        <v>1.9938461538461541E-11</v>
+        <v>4.8703846153846161E-10</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -1811,7 +1818,7 @@
         <v>55</v>
       </c>
       <c r="B106" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C106">
         <v>1.9938461538461541E-11</v>
@@ -1822,7 +1829,7 @@
         <v>55</v>
       </c>
       <c r="B107" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C107">
         <v>1.9938461538461541E-11</v>
@@ -1833,7 +1840,7 @@
         <v>55</v>
       </c>
       <c r="B108" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C108">
         <v>1.9938461538461541E-11</v>
@@ -1841,24 +1848,24 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C109">
-        <v>1.3188461538461541E-10</v>
+        <v>1.9938461538461541E-11</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C110">
-        <v>1.3188461538461541E-10</v>
+        <v>1.9938461538461541E-11</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -1866,7 +1873,7 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C111">
         <v>1.3188461538461541E-10</v>
@@ -1877,7 +1884,7 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C112">
         <v>1.3188461538461541E-10</v>
@@ -1888,7 +1895,7 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C113">
         <v>1.3188461538461541E-10</v>
@@ -1896,24 +1903,24 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C114">
-        <v>1.7687076923076921E-9</v>
+        <v>1.3188461538461541E-10</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C115">
-        <v>1.7687076923076921E-9</v>
+        <v>1.3188461538461541E-10</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -1921,7 +1928,7 @@
         <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C116">
         <v>1.7687076923076921E-9</v>
@@ -1932,7 +1939,7 @@
         <v>57</v>
       </c>
       <c r="B117" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C117">
         <v>1.7687076923076921E-9</v>
@@ -1943,7 +1950,7 @@
         <v>57</v>
       </c>
       <c r="B118" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C118">
         <v>1.7687076923076921E-9</v>
@@ -1951,24 +1958,24 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C119">
-        <v>2.5629230769230769E-9</v>
+        <v>1.7687076923076921E-9</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B120" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C120">
-        <v>2.5629230769230769E-9</v>
+        <v>1.7687076923076921E-9</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -1976,7 +1983,7 @@
         <v>58</v>
       </c>
       <c r="B121" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C121">
         <v>2.5629230769230769E-9</v>
@@ -1987,7 +1994,7 @@
         <v>58</v>
       </c>
       <c r="B122" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C122">
         <v>2.5629230769230769E-9</v>
@@ -1998,7 +2005,7 @@
         <v>58</v>
       </c>
       <c r="B123" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C123">
         <v>2.5629230769230769E-9</v>
@@ -2006,24 +2013,24 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B124" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C124">
-        <v>7.6659230769230773E-10</v>
+        <v>2.5629230769230769E-9</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B125" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C125">
-        <v>7.6659230769230773E-10</v>
+        <v>2.5629230769230769E-9</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -2031,7 +2038,7 @@
         <v>59</v>
       </c>
       <c r="B126" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C126">
         <v>7.6659230769230773E-10</v>
@@ -2042,7 +2049,7 @@
         <v>59</v>
       </c>
       <c r="B127" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C127">
         <v>7.6659230769230773E-10</v>
@@ -2053,7 +2060,7 @@
         <v>59</v>
       </c>
       <c r="B128" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C128">
         <v>7.6659230769230773E-10</v>
@@ -2061,35 +2068,35 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="B129" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C129">
-        <v>7.4769230769230768E-12</v>
+        <v>7.6659230769230773E-10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B130" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C130">
-        <v>6.2307692307692306E-13</v>
+        <v>7.6659230769230773E-10</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B131" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C131">
-        <v>6.2307692307692306E-13</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -2097,7 +2104,7 @@
         <v>60</v>
       </c>
       <c r="B132" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C132">
         <v>6.2307692307692306E-13</v>
@@ -2108,7 +2115,7 @@
         <v>60</v>
       </c>
       <c r="B133" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C133">
         <v>6.2307692307692306E-13</v>
@@ -2119,7 +2126,7 @@
         <v>60</v>
       </c>
       <c r="B134" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C134">
         <v>6.2307692307692306E-13</v>
@@ -2127,24 +2134,24 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B135" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C135">
-        <v>4.29923076923077E-10</v>
+        <v>6.2307692307692306E-13</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B136" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C136">
-        <v>4.29923076923077E-10</v>
+        <v>6.2307692307692306E-13</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -2152,7 +2159,7 @@
         <v>61</v>
       </c>
       <c r="B137" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C137">
         <v>4.29923076923077E-10</v>
@@ -2163,7 +2170,7 @@
         <v>61</v>
       </c>
       <c r="B138" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C138">
         <v>4.29923076923077E-10</v>
@@ -2174,7 +2181,7 @@
         <v>61</v>
       </c>
       <c r="B139" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C139">
         <v>4.29923076923077E-10</v>
@@ -2182,24 +2189,24 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B140" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C140">
-        <v>1.4858307692307699E-9</v>
+        <v>4.29923076923077E-10</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B141" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C141">
-        <v>1.4858307692307699E-9</v>
+        <v>4.29923076923077E-10</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -2207,7 +2214,7 @@
         <v>62</v>
       </c>
       <c r="B142" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C142">
         <v>1.4858307692307699E-9</v>
@@ -2218,7 +2225,7 @@
         <v>62</v>
       </c>
       <c r="B143" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C143">
         <v>1.4858307692307699E-9</v>
@@ -2229,7 +2236,7 @@
         <v>62</v>
       </c>
       <c r="B144" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C144">
         <v>1.4858307692307699E-9</v>
@@ -2237,24 +2244,24 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B145" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C145">
-        <v>4.3740000000000001E-10</v>
+        <v>1.4858307692307699E-9</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B146" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C146">
-        <v>4.3740000000000001E-10</v>
+        <v>1.4858307692307699E-9</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2262,7 +2269,7 @@
         <v>63</v>
       </c>
       <c r="B147" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C147">
         <v>4.3740000000000001E-10</v>
@@ -2273,7 +2280,7 @@
         <v>63</v>
       </c>
       <c r="B148" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C148">
         <v>4.3740000000000001E-10</v>
@@ -2284,7 +2291,7 @@
         <v>63</v>
       </c>
       <c r="B149" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C149">
         <v>4.3740000000000001E-10</v>
@@ -2292,24 +2299,24 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B150" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C150">
-        <v>3.2090538461538469E-9</v>
+        <v>4.3740000000000001E-10</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B151" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C151">
-        <v>3.2090538461538469E-9</v>
+        <v>4.3740000000000001E-10</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -2317,7 +2324,7 @@
         <v>64</v>
       </c>
       <c r="B152" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C152">
         <v>3.2090538461538469E-9</v>
@@ -2328,7 +2335,7 @@
         <v>64</v>
       </c>
       <c r="B153" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C153">
         <v>3.2090538461538469E-9</v>
@@ -2339,7 +2346,7 @@
         <v>64</v>
       </c>
       <c r="B154" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C154">
         <v>3.2090538461538469E-9</v>
@@ -2347,24 +2354,24 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B155" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C155">
-        <v>2.2846153846153851E-12</v>
+        <v>3.2090538461538469E-9</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B156" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C156">
-        <v>2.2846153846153851E-12</v>
+        <v>3.2090538461538469E-9</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -2372,7 +2379,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C157">
         <v>2.2846153846153851E-12</v>
@@ -2383,7 +2390,7 @@
         <v>65</v>
       </c>
       <c r="B158" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C158">
         <v>2.2846153846153851E-12</v>
@@ -2394,7 +2401,7 @@
         <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C159">
         <v>2.2846153846153851E-12</v>
@@ -2402,24 +2409,24 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B160" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C160">
-        <v>2.3982230769230768E-9</v>
+        <v>2.2846153846153851E-12</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B161" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C161">
-        <v>2.3982230769230768E-9</v>
+        <v>2.2846153846153851E-12</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -2427,7 +2434,7 @@
         <v>66</v>
       </c>
       <c r="B162" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C162">
         <v>2.3982230769230768E-9</v>
@@ -2438,7 +2445,7 @@
         <v>66</v>
       </c>
       <c r="B163" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C163">
         <v>2.3982230769230768E-9</v>
@@ -2449,7 +2456,7 @@
         <v>66</v>
       </c>
       <c r="B164" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C164">
         <v>2.3982230769230768E-9</v>
@@ -2457,24 +2464,24 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B165" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C165">
-        <v>3.7176923076923081E-11</v>
+        <v>2.3982230769230768E-9</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B166" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C166">
-        <v>3.7176923076923081E-11</v>
+        <v>2.3982230769230768E-9</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -2482,7 +2489,7 @@
         <v>67</v>
       </c>
       <c r="B167" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C167">
         <v>3.7176923076923081E-11</v>
@@ -2493,7 +2500,7 @@
         <v>67</v>
       </c>
       <c r="B168" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C168">
         <v>3.7176923076923081E-11</v>
@@ -2504,7 +2511,7 @@
         <v>67</v>
       </c>
       <c r="B169" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C169">
         <v>3.7176923076923081E-11</v>
@@ -2512,24 +2519,24 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B170" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C170">
-        <v>1.6968461538461539E-10</v>
+        <v>3.7176923076923081E-11</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B171" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C171">
-        <v>1.6968461538461539E-10</v>
+        <v>3.7176923076923081E-11</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -2537,7 +2544,7 @@
         <v>68</v>
       </c>
       <c r="B172" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C172">
         <v>1.6968461538461539E-10</v>
@@ -2548,7 +2555,7 @@
         <v>68</v>
       </c>
       <c r="B173" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C173">
         <v>1.6968461538461539E-10</v>
@@ -2559,7 +2566,7 @@
         <v>68</v>
       </c>
       <c r="B174" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C174">
         <v>1.6968461538461539E-10</v>
@@ -2567,24 +2574,24 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B175" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C175">
-        <v>7.4769230769230768E-12</v>
+        <v>1.6968461538461539E-10</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B176" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C176">
-        <v>7.4769230769230768E-12</v>
+        <v>1.6968461538461539E-10</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -2592,7 +2599,7 @@
         <v>69</v>
       </c>
       <c r="B177" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C177">
         <v>7.4769230769230768E-12</v>
@@ -2603,7 +2610,7 @@
         <v>69</v>
       </c>
       <c r="B178" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C178">
         <v>7.4769230769230768E-12</v>
@@ -2614,7 +2621,7 @@
         <v>69</v>
       </c>
       <c r="B179" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C179">
         <v>7.4769230769230768E-12</v>
@@ -2622,24 +2629,24 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B180" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C180">
-        <v>7.0615384615384616E-12</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B181" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C181">
-        <v>7.0615384615384616E-12</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -2647,7 +2654,7 @@
         <v>70</v>
       </c>
       <c r="B182" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C182">
         <v>7.0615384615384616E-12</v>
@@ -2658,7 +2665,7 @@
         <v>70</v>
       </c>
       <c r="B183" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C183">
         <v>7.0615384615384616E-12</v>
@@ -2669,7 +2676,7 @@
         <v>70</v>
       </c>
       <c r="B184" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C184">
         <v>7.0615384615384616E-12</v>
@@ -2680,7 +2687,7 @@
         <v>70</v>
       </c>
       <c r="B185" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C185">
         <v>7.0615384615384616E-12</v>
@@ -2688,24 +2695,24 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B186" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C186">
-        <v>3.1153846153846161E-12</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B187" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C187">
-        <v>3.1153846153846161E-12</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -2713,7 +2720,7 @@
         <v>71</v>
       </c>
       <c r="B188" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C188">
         <v>3.1153846153846161E-12</v>
@@ -2724,7 +2731,7 @@
         <v>71</v>
       </c>
       <c r="B189" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C189">
         <v>3.1153846153846161E-12</v>
@@ -2735,7 +2742,7 @@
         <v>71</v>
       </c>
       <c r="B190" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C190">
         <v>3.1153846153846161E-12</v>
@@ -2743,24 +2750,24 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B191" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C191">
-        <v>7.0615384615384616E-12</v>
+        <v>3.1153846153846161E-12</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B192" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C192">
-        <v>7.0615384615384616E-12</v>
+        <v>3.1153846153846161E-12</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -2768,7 +2775,7 @@
         <v>72</v>
       </c>
       <c r="B193" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C193">
         <v>7.0615384615384616E-12</v>
@@ -2779,7 +2786,7 @@
         <v>72</v>
       </c>
       <c r="B194" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C194">
         <v>7.0615384615384616E-12</v>
@@ -2790,7 +2797,7 @@
         <v>72</v>
       </c>
       <c r="B195" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C195">
         <v>7.0615384615384616E-12</v>
@@ -2798,24 +2805,24 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B196" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C196">
-        <v>4.1933076923076919E-10</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B197" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C197">
-        <v>4.1933076923076919E-10</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -2823,7 +2830,7 @@
         <v>73</v>
       </c>
       <c r="B198" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C198">
         <v>4.1933076923076919E-10</v>
@@ -2834,7 +2841,7 @@
         <v>73</v>
       </c>
       <c r="B199" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C199">
         <v>4.1933076923076919E-10</v>
@@ -2845,7 +2852,7 @@
         <v>73</v>
       </c>
       <c r="B200" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C200">
         <v>4.1933076923076919E-10</v>
@@ -2853,24 +2860,24 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B201" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C201">
-        <v>1.5263307692307689E-9</v>
+        <v>4.1933076923076919E-10</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B202" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C202">
-        <v>1.5263307692307689E-9</v>
+        <v>4.1933076923076919E-10</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -2878,7 +2885,7 @@
         <v>74</v>
       </c>
       <c r="B203" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C203">
         <v>1.5263307692307689E-9</v>
@@ -2889,7 +2896,7 @@
         <v>74</v>
       </c>
       <c r="B204" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C204">
         <v>1.5263307692307689E-9</v>
@@ -2900,7 +2907,7 @@
         <v>74</v>
       </c>
       <c r="B205" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C205">
         <v>1.5263307692307689E-9</v>
@@ -2908,24 +2915,24 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B206" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C206">
-        <v>1.111569230769231E-9</v>
+        <v>1.5263307692307689E-9</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B207" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C207">
-        <v>1.111569230769231E-9</v>
+        <v>1.5263307692307689E-9</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -2933,7 +2940,7 @@
         <v>75</v>
       </c>
       <c r="B208" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C208">
         <v>1.111569230769231E-9</v>
@@ -2944,7 +2951,7 @@
         <v>75</v>
       </c>
       <c r="B209" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C209">
         <v>1.111569230769231E-9</v>
@@ -2955,7 +2962,7 @@
         <v>75</v>
       </c>
       <c r="B210" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C210">
         <v>1.111569230769231E-9</v>
@@ -2963,24 +2970,24 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B211" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C211">
-        <v>2.8777846153846162E-9</v>
+        <v>1.111569230769231E-9</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B212" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C212">
-        <v>2.8777846153846162E-9</v>
+        <v>1.111569230769231E-9</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -2988,7 +2995,7 @@
         <v>76</v>
       </c>
       <c r="B213" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C213">
         <v>2.8777846153846162E-9</v>
@@ -2999,7 +3006,7 @@
         <v>76</v>
       </c>
       <c r="B214" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C214">
         <v>2.8777846153846162E-9</v>
@@ -3010,7 +3017,7 @@
         <v>76</v>
       </c>
       <c r="B215" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C215">
         <v>2.8777846153846162E-9</v>
@@ -3018,24 +3025,24 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B216" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C216">
-        <v>3.714576923076923E-9</v>
+        <v>2.8777846153846162E-9</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B217" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C217">
-        <v>3.714576923076923E-9</v>
+        <v>2.8777846153846162E-9</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
@@ -3043,7 +3050,7 @@
         <v>77</v>
       </c>
       <c r="B218" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C218">
         <v>3.714576923076923E-9</v>
@@ -3054,7 +3061,7 @@
         <v>77</v>
       </c>
       <c r="B219" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C219">
         <v>3.714576923076923E-9</v>
@@ -3065,7 +3072,7 @@
         <v>77</v>
       </c>
       <c r="B220" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C220">
         <v>3.714576923076923E-9</v>
@@ -3073,35 +3080,35 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B221" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C221">
-        <v>1.969753846153846E-9</v>
+        <v>3.714576923076923E-9</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B222" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C222">
-        <v>5.418069230769231E-9</v>
+        <v>3.714576923076923E-9</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B223" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C223">
-        <v>5.418069230769231E-9</v>
+        <v>1.969753846153846E-9</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
@@ -3109,7 +3116,7 @@
         <v>79</v>
       </c>
       <c r="B224" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C224">
         <v>5.418069230769231E-9</v>
@@ -3120,7 +3127,7 @@
         <v>79</v>
       </c>
       <c r="B225" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C225">
         <v>5.418069230769231E-9</v>
@@ -3131,9 +3138,31 @@
         <v>79</v>
       </c>
       <c r="B226" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C226">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>79</v>
+      </c>
+      <c r="B227" t="s">
+        <v>85</v>
+      </c>
+      <c r="C227">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>79</v>
+      </c>
+      <c r="B228" t="s">
+        <v>82</v>
+      </c>
+      <c r="C228">
         <v>5.418069230769231E-9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove CF "Occupation, water courses, artificial"
"Occupation, water courses, artificial" (natural resource::land) does not exist in ecoinvent nomenclature.

IMO: "Occupation, water courses, artificial" in simapro should map to "Occupation, river, artificial" and "Occupation, lakes, artificial"
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC7313-380C-4585-81B9-173E4CE37D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1708E204-E421-4F5C-9C25-D14AA61620AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="91">
   <si>
     <t>name</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>Occupation, lakes, artificial</t>
-  </si>
-  <si>
-    <t>Occupation, water courses, artificial</t>
   </si>
 </sst>
 </file>
@@ -644,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,30 +997,30 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="2">
-        <v>7.6923076923076923E-13</v>
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>80</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>7.3076923076923074E-13</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>80</v>
@@ -1034,7 +1031,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>80</v>
@@ -1045,7 +1042,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>80</v>
@@ -1056,7 +1053,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>80</v>
@@ -1067,7 +1064,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>80</v>
@@ -1078,7 +1075,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>80</v>
@@ -1089,13 +1086,13 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C40">
-        <v>7.3076923076923074E-13</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1103,7 +1100,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <v>4.1538461538461543E-12</v>
@@ -1114,7 +1111,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42">
         <v>4.1538461538461543E-12</v>
@@ -1125,7 +1122,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43">
         <v>4.1538461538461543E-12</v>
@@ -1136,7 +1133,7 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C44">
         <v>4.1538461538461543E-12</v>
@@ -1144,13 +1141,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C45">
-        <v>4.1538461538461543E-12</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1158,7 +1155,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C46">
         <v>2.8661538461538461E-12</v>
@@ -1169,7 +1166,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C47">
         <v>2.8661538461538461E-12</v>
@@ -1180,7 +1177,7 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C48">
         <v>2.8661538461538461E-12</v>
@@ -1191,7 +1188,7 @@
         <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C49">
         <v>2.8661538461538461E-12</v>
@@ -1199,13 +1196,13 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C50">
-        <v>2.8661538461538461E-12</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1213,7 +1210,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C51">
         <v>2.076923076923077E-13</v>
@@ -1224,7 +1221,7 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C52">
         <v>2.076923076923077E-13</v>
@@ -1235,7 +1232,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C53">
         <v>2.076923076923077E-13</v>
@@ -1246,7 +1243,7 @@
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C54">
         <v>2.076923076923077E-13</v>
@@ -1254,10 +1251,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C55">
         <v>2.076923076923077E-13</v>
@@ -1268,7 +1265,7 @@
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C56">
         <v>2.076923076923077E-13</v>
@@ -1279,7 +1276,7 @@
         <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C57">
         <v>2.076923076923077E-13</v>
@@ -1290,7 +1287,7 @@
         <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C58">
         <v>2.076923076923077E-13</v>
@@ -1301,7 +1298,7 @@
         <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C59">
         <v>2.076923076923077E-13</v>
@@ -1312,7 +1309,7 @@
         <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C60">
         <v>2.076923076923077E-13</v>
@@ -1320,13 +1317,13 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C61">
-        <v>2.076923076923077E-13</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1334,7 +1331,7 @@
         <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C62">
         <v>-2.076923076923077E-13</v>
@@ -1345,7 +1342,7 @@
         <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C63">
         <v>-2.076923076923077E-13</v>
@@ -1356,7 +1353,7 @@
         <v>45</v>
       </c>
       <c r="B64" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C64">
         <v>-2.076923076923077E-13</v>
@@ -1364,13 +1361,13 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="C65">
-        <v>-2.076923076923077E-13</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1378,7 +1375,7 @@
         <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C66">
         <v>6.1892307692307702E-11</v>
@@ -1389,7 +1386,7 @@
         <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C67">
         <v>6.1892307692307702E-11</v>
@@ -1400,7 +1397,7 @@
         <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C68">
         <v>6.1892307692307702E-11</v>
@@ -1411,7 +1408,7 @@
         <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C69">
         <v>6.1892307692307702E-11</v>
@@ -1419,13 +1416,13 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C70">
-        <v>6.1892307692307702E-11</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1433,7 +1430,7 @@
         <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C71">
         <v>3.2171538461538461E-10</v>
@@ -1444,7 +1441,7 @@
         <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C72">
         <v>3.2171538461538461E-10</v>
@@ -1455,7 +1452,7 @@
         <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C73">
         <v>3.2171538461538461E-10</v>
@@ -1466,7 +1463,7 @@
         <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C74">
         <v>3.2171538461538461E-10</v>
@@ -1474,13 +1471,13 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C75">
-        <v>3.2171538461538461E-10</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1488,7 +1485,7 @@
         <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C76">
         <v>1.143969230769231E-9</v>
@@ -1499,7 +1496,7 @@
         <v>49</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C77">
         <v>1.143969230769231E-9</v>
@@ -1510,7 +1507,7 @@
         <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C78">
         <v>1.143969230769231E-9</v>
@@ -1521,7 +1518,7 @@
         <v>49</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C79">
         <v>1.143969230769231E-9</v>
@@ -1529,13 +1526,13 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C80">
-        <v>1.143969230769231E-9</v>
+        <v>1.3678615384615381E-9</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1543,7 +1540,7 @@
         <v>50</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C81">
         <v>1.3678615384615381E-9</v>
@@ -1554,7 +1551,7 @@
         <v>50</v>
       </c>
       <c r="B82" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C82">
         <v>1.3678615384615381E-9</v>
@@ -1565,7 +1562,7 @@
         <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C83">
         <v>1.3678615384615381E-9</v>
@@ -1576,7 +1573,7 @@
         <v>50</v>
       </c>
       <c r="B84" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C84">
         <v>1.3678615384615381E-9</v>
@@ -1584,13 +1581,13 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C85">
-        <v>1.3678615384615381E-9</v>
+        <v>1.9481538461538459E-10</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -1598,7 +1595,7 @@
         <v>51</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C86">
         <v>1.9481538461538459E-10</v>
@@ -1609,7 +1606,7 @@
         <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C87">
         <v>1.9481538461538459E-10</v>
@@ -1620,7 +1617,7 @@
         <v>51</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C88">
         <v>1.9481538461538459E-10</v>
@@ -1631,7 +1628,7 @@
         <v>51</v>
       </c>
       <c r="B89" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C89">
         <v>1.9481538461538459E-10</v>
@@ -1639,13 +1636,13 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C90">
-        <v>1.9481538461538459E-10</v>
+        <v>3.4684615384615383E-11</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -1653,7 +1650,7 @@
         <v>52</v>
       </c>
       <c r="B91" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C91">
         <v>3.4684615384615383E-11</v>
@@ -1664,7 +1661,7 @@
         <v>52</v>
       </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C92">
         <v>3.4684615384615383E-11</v>
@@ -1675,7 +1672,7 @@
         <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C93">
         <v>3.4684615384615383E-11</v>
@@ -1686,7 +1683,7 @@
         <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C94">
         <v>3.4684615384615383E-11</v>
@@ -1694,13 +1691,13 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C95">
-        <v>3.4684615384615383E-11</v>
+        <v>1.9969615384615379E-9</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -1708,7 +1705,7 @@
         <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C96">
         <v>1.9969615384615379E-9</v>
@@ -1719,7 +1716,7 @@
         <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C97">
         <v>1.9969615384615379E-9</v>
@@ -1730,7 +1727,7 @@
         <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C98">
         <v>1.9969615384615379E-9</v>
@@ -1741,7 +1738,7 @@
         <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C99">
         <v>1.9969615384615379E-9</v>
@@ -1749,13 +1746,13 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B100" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C100">
-        <v>1.9969615384615379E-9</v>
+        <v>4.8703846153846161E-10</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1763,7 +1760,7 @@
         <v>54</v>
       </c>
       <c r="B101" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C101">
         <v>4.8703846153846161E-10</v>
@@ -1774,7 +1771,7 @@
         <v>54</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C102">
         <v>4.8703846153846161E-10</v>
@@ -1785,7 +1782,7 @@
         <v>54</v>
       </c>
       <c r="B103" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C103">
         <v>4.8703846153846161E-10</v>
@@ -1796,7 +1793,7 @@
         <v>54</v>
       </c>
       <c r="B104" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C104">
         <v>4.8703846153846161E-10</v>
@@ -1804,13 +1801,13 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B105" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C105">
-        <v>4.8703846153846161E-10</v>
+        <v>1.9938461538461541E-11</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -1818,7 +1815,7 @@
         <v>55</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C106">
         <v>1.9938461538461541E-11</v>
@@ -1829,7 +1826,7 @@
         <v>55</v>
       </c>
       <c r="B107" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C107">
         <v>1.9938461538461541E-11</v>
@@ -1840,7 +1837,7 @@
         <v>55</v>
       </c>
       <c r="B108" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C108">
         <v>1.9938461538461541E-11</v>
@@ -1851,7 +1848,7 @@
         <v>55</v>
       </c>
       <c r="B109" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C109">
         <v>1.9938461538461541E-11</v>
@@ -1859,13 +1856,13 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C110">
-        <v>1.9938461538461541E-11</v>
+        <v>1.3188461538461541E-10</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -1873,7 +1870,7 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C111">
         <v>1.3188461538461541E-10</v>
@@ -1884,7 +1881,7 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C112">
         <v>1.3188461538461541E-10</v>
@@ -1895,7 +1892,7 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C113">
         <v>1.3188461538461541E-10</v>
@@ -1906,7 +1903,7 @@
         <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C114">
         <v>1.3188461538461541E-10</v>
@@ -1914,13 +1911,13 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B115" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C115">
-        <v>1.3188461538461541E-10</v>
+        <v>1.7687076923076921E-9</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -1928,7 +1925,7 @@
         <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C116">
         <v>1.7687076923076921E-9</v>
@@ -1939,7 +1936,7 @@
         <v>57</v>
       </c>
       <c r="B117" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C117">
         <v>1.7687076923076921E-9</v>
@@ -1950,7 +1947,7 @@
         <v>57</v>
       </c>
       <c r="B118" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C118">
         <v>1.7687076923076921E-9</v>
@@ -1961,7 +1958,7 @@
         <v>57</v>
       </c>
       <c r="B119" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C119">
         <v>1.7687076923076921E-9</v>
@@ -1969,13 +1966,13 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B120" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C120">
-        <v>1.7687076923076921E-9</v>
+        <v>2.5629230769230769E-9</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -1983,7 +1980,7 @@
         <v>58</v>
       </c>
       <c r="B121" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C121">
         <v>2.5629230769230769E-9</v>
@@ -1994,7 +1991,7 @@
         <v>58</v>
       </c>
       <c r="B122" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C122">
         <v>2.5629230769230769E-9</v>
@@ -2005,7 +2002,7 @@
         <v>58</v>
       </c>
       <c r="B123" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C123">
         <v>2.5629230769230769E-9</v>
@@ -2016,7 +2013,7 @@
         <v>58</v>
       </c>
       <c r="B124" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C124">
         <v>2.5629230769230769E-9</v>
@@ -2024,13 +2021,13 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B125" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C125">
-        <v>2.5629230769230769E-9</v>
+        <v>7.6659230769230773E-10</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -2038,7 +2035,7 @@
         <v>59</v>
       </c>
       <c r="B126" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C126">
         <v>7.6659230769230773E-10</v>
@@ -2049,7 +2046,7 @@
         <v>59</v>
       </c>
       <c r="B127" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C127">
         <v>7.6659230769230773E-10</v>
@@ -2060,7 +2057,7 @@
         <v>59</v>
       </c>
       <c r="B128" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C128">
         <v>7.6659230769230773E-10</v>
@@ -2071,7 +2068,7 @@
         <v>59</v>
       </c>
       <c r="B129" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C129">
         <v>7.6659230769230773E-10</v>
@@ -2079,24 +2076,24 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B130" t="s">
         <v>82</v>
       </c>
       <c r="C130">
-        <v>7.6659230769230773E-10</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B131" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C131">
-        <v>7.4769230769230768E-12</v>
+        <v>6.2307692307692306E-13</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -2104,7 +2101,7 @@
         <v>60</v>
       </c>
       <c r="B132" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C132">
         <v>6.2307692307692306E-13</v>
@@ -2115,7 +2112,7 @@
         <v>60</v>
       </c>
       <c r="B133" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C133">
         <v>6.2307692307692306E-13</v>
@@ -2126,7 +2123,7 @@
         <v>60</v>
       </c>
       <c r="B134" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C134">
         <v>6.2307692307692306E-13</v>
@@ -2137,7 +2134,7 @@
         <v>60</v>
       </c>
       <c r="B135" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C135">
         <v>6.2307692307692306E-13</v>
@@ -2145,13 +2142,13 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B136" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C136">
-        <v>6.2307692307692306E-13</v>
+        <v>4.29923076923077E-10</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -2159,7 +2156,7 @@
         <v>61</v>
       </c>
       <c r="B137" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C137">
         <v>4.29923076923077E-10</v>
@@ -2170,7 +2167,7 @@
         <v>61</v>
       </c>
       <c r="B138" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C138">
         <v>4.29923076923077E-10</v>
@@ -2181,7 +2178,7 @@
         <v>61</v>
       </c>
       <c r="B139" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C139">
         <v>4.29923076923077E-10</v>
@@ -2192,7 +2189,7 @@
         <v>61</v>
       </c>
       <c r="B140" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C140">
         <v>4.29923076923077E-10</v>
@@ -2200,13 +2197,13 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B141" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C141">
-        <v>4.29923076923077E-10</v>
+        <v>1.4858307692307699E-9</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -2214,7 +2211,7 @@
         <v>62</v>
       </c>
       <c r="B142" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C142">
         <v>1.4858307692307699E-9</v>
@@ -2225,7 +2222,7 @@
         <v>62</v>
       </c>
       <c r="B143" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C143">
         <v>1.4858307692307699E-9</v>
@@ -2236,7 +2233,7 @@
         <v>62</v>
       </c>
       <c r="B144" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C144">
         <v>1.4858307692307699E-9</v>
@@ -2247,7 +2244,7 @@
         <v>62</v>
       </c>
       <c r="B145" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C145">
         <v>1.4858307692307699E-9</v>
@@ -2255,13 +2252,13 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B146" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C146">
-        <v>1.4858307692307699E-9</v>
+        <v>4.3740000000000001E-10</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2269,7 +2266,7 @@
         <v>63</v>
       </c>
       <c r="B147" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C147">
         <v>4.3740000000000001E-10</v>
@@ -2280,7 +2277,7 @@
         <v>63</v>
       </c>
       <c r="B148" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C148">
         <v>4.3740000000000001E-10</v>
@@ -2291,7 +2288,7 @@
         <v>63</v>
       </c>
       <c r="B149" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C149">
         <v>4.3740000000000001E-10</v>
@@ -2302,7 +2299,7 @@
         <v>63</v>
       </c>
       <c r="B150" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C150">
         <v>4.3740000000000001E-10</v>
@@ -2310,13 +2307,13 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B151" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C151">
-        <v>4.3740000000000001E-10</v>
+        <v>3.2090538461538469E-9</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -2324,7 +2321,7 @@
         <v>64</v>
       </c>
       <c r="B152" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C152">
         <v>3.2090538461538469E-9</v>
@@ -2335,7 +2332,7 @@
         <v>64</v>
       </c>
       <c r="B153" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C153">
         <v>3.2090538461538469E-9</v>
@@ -2346,7 +2343,7 @@
         <v>64</v>
       </c>
       <c r="B154" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C154">
         <v>3.2090538461538469E-9</v>
@@ -2357,7 +2354,7 @@
         <v>64</v>
       </c>
       <c r="B155" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C155">
         <v>3.2090538461538469E-9</v>
@@ -2365,13 +2362,13 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B156" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C156">
-        <v>3.2090538461538469E-9</v>
+        <v>2.2846153846153851E-12</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -2379,7 +2376,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C157">
         <v>2.2846153846153851E-12</v>
@@ -2390,7 +2387,7 @@
         <v>65</v>
       </c>
       <c r="B158" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C158">
         <v>2.2846153846153851E-12</v>
@@ -2401,7 +2398,7 @@
         <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C159">
         <v>2.2846153846153851E-12</v>
@@ -2412,7 +2409,7 @@
         <v>65</v>
       </c>
       <c r="B160" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C160">
         <v>2.2846153846153851E-12</v>
@@ -2420,13 +2417,13 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B161" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C161">
-        <v>2.2846153846153851E-12</v>
+        <v>2.3982230769230768E-9</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -2434,7 +2431,7 @@
         <v>66</v>
       </c>
       <c r="B162" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C162">
         <v>2.3982230769230768E-9</v>
@@ -2445,7 +2442,7 @@
         <v>66</v>
       </c>
       <c r="B163" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C163">
         <v>2.3982230769230768E-9</v>
@@ -2456,7 +2453,7 @@
         <v>66</v>
       </c>
       <c r="B164" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C164">
         <v>2.3982230769230768E-9</v>
@@ -2467,7 +2464,7 @@
         <v>66</v>
       </c>
       <c r="B165" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C165">
         <v>2.3982230769230768E-9</v>
@@ -2475,13 +2472,13 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B166" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C166">
-        <v>2.3982230769230768E-9</v>
+        <v>3.7176923076923081E-11</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -2489,7 +2486,7 @@
         <v>67</v>
       </c>
       <c r="B167" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C167">
         <v>3.7176923076923081E-11</v>
@@ -2500,7 +2497,7 @@
         <v>67</v>
       </c>
       <c r="B168" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C168">
         <v>3.7176923076923081E-11</v>
@@ -2511,7 +2508,7 @@
         <v>67</v>
       </c>
       <c r="B169" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C169">
         <v>3.7176923076923081E-11</v>
@@ -2522,7 +2519,7 @@
         <v>67</v>
       </c>
       <c r="B170" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C170">
         <v>3.7176923076923081E-11</v>
@@ -2530,13 +2527,13 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B171" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C171">
-        <v>3.7176923076923081E-11</v>
+        <v>1.6968461538461539E-10</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -2544,7 +2541,7 @@
         <v>68</v>
       </c>
       <c r="B172" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C172">
         <v>1.6968461538461539E-10</v>
@@ -2555,7 +2552,7 @@
         <v>68</v>
       </c>
       <c r="B173" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C173">
         <v>1.6968461538461539E-10</v>
@@ -2566,7 +2563,7 @@
         <v>68</v>
       </c>
       <c r="B174" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C174">
         <v>1.6968461538461539E-10</v>
@@ -2577,7 +2574,7 @@
         <v>68</v>
       </c>
       <c r="B175" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C175">
         <v>1.6968461538461539E-10</v>
@@ -2585,13 +2582,13 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B176" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C176">
-        <v>1.6968461538461539E-10</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -2599,7 +2596,7 @@
         <v>69</v>
       </c>
       <c r="B177" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C177">
         <v>7.4769230769230768E-12</v>
@@ -2610,7 +2607,7 @@
         <v>69</v>
       </c>
       <c r="B178" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C178">
         <v>7.4769230769230768E-12</v>
@@ -2621,7 +2618,7 @@
         <v>69</v>
       </c>
       <c r="B179" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C179">
         <v>7.4769230769230768E-12</v>
@@ -2632,7 +2629,7 @@
         <v>69</v>
       </c>
       <c r="B180" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C180">
         <v>7.4769230769230768E-12</v>
@@ -2640,13 +2637,13 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B181" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C181">
-        <v>7.4769230769230768E-12</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -2654,7 +2651,7 @@
         <v>70</v>
       </c>
       <c r="B182" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C182">
         <v>7.0615384615384616E-12</v>
@@ -2665,7 +2662,7 @@
         <v>70</v>
       </c>
       <c r="B183" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C183">
         <v>7.0615384615384616E-12</v>
@@ -2676,7 +2673,7 @@
         <v>70</v>
       </c>
       <c r="B184" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C184">
         <v>7.0615384615384616E-12</v>
@@ -2687,7 +2684,7 @@
         <v>70</v>
       </c>
       <c r="B185" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C185">
         <v>7.0615384615384616E-12</v>
@@ -2698,7 +2695,7 @@
         <v>70</v>
       </c>
       <c r="B186" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C186">
         <v>7.0615384615384616E-12</v>
@@ -2706,13 +2703,13 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B187" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="C187">
-        <v>7.0615384615384616E-12</v>
+        <v>3.1153846153846161E-12</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -2720,7 +2717,7 @@
         <v>71</v>
       </c>
       <c r="B188" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C188">
         <v>3.1153846153846161E-12</v>
@@ -2731,7 +2728,7 @@
         <v>71</v>
       </c>
       <c r="B189" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C189">
         <v>3.1153846153846161E-12</v>
@@ -2742,7 +2739,7 @@
         <v>71</v>
       </c>
       <c r="B190" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C190">
         <v>3.1153846153846161E-12</v>
@@ -2753,7 +2750,7 @@
         <v>71</v>
       </c>
       <c r="B191" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C191">
         <v>3.1153846153846161E-12</v>
@@ -2761,13 +2758,13 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B192" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C192">
-        <v>3.1153846153846161E-12</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -2775,7 +2772,7 @@
         <v>72</v>
       </c>
       <c r="B193" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C193">
         <v>7.0615384615384616E-12</v>
@@ -2786,7 +2783,7 @@
         <v>72</v>
       </c>
       <c r="B194" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C194">
         <v>7.0615384615384616E-12</v>
@@ -2797,7 +2794,7 @@
         <v>72</v>
       </c>
       <c r="B195" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C195">
         <v>7.0615384615384616E-12</v>
@@ -2808,7 +2805,7 @@
         <v>72</v>
       </c>
       <c r="B196" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C196">
         <v>7.0615384615384616E-12</v>
@@ -2816,13 +2813,13 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B197" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C197">
-        <v>7.0615384615384616E-12</v>
+        <v>4.1933076923076919E-10</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -2830,7 +2827,7 @@
         <v>73</v>
       </c>
       <c r="B198" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C198">
         <v>4.1933076923076919E-10</v>
@@ -2841,7 +2838,7 @@
         <v>73</v>
       </c>
       <c r="B199" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C199">
         <v>4.1933076923076919E-10</v>
@@ -2852,7 +2849,7 @@
         <v>73</v>
       </c>
       <c r="B200" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C200">
         <v>4.1933076923076919E-10</v>
@@ -2863,7 +2860,7 @@
         <v>73</v>
       </c>
       <c r="B201" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C201">
         <v>4.1933076923076919E-10</v>
@@ -2871,13 +2868,13 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B202" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C202">
-        <v>4.1933076923076919E-10</v>
+        <v>1.5263307692307689E-9</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -2885,7 +2882,7 @@
         <v>74</v>
       </c>
       <c r="B203" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C203">
         <v>1.5263307692307689E-9</v>
@@ -2896,7 +2893,7 @@
         <v>74</v>
       </c>
       <c r="B204" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C204">
         <v>1.5263307692307689E-9</v>
@@ -2907,7 +2904,7 @@
         <v>74</v>
       </c>
       <c r="B205" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C205">
         <v>1.5263307692307689E-9</v>
@@ -2918,7 +2915,7 @@
         <v>74</v>
       </c>
       <c r="B206" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C206">
         <v>1.5263307692307689E-9</v>
@@ -2926,13 +2923,13 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B207" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C207">
-        <v>1.5263307692307689E-9</v>
+        <v>1.111569230769231E-9</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -2940,7 +2937,7 @@
         <v>75</v>
       </c>
       <c r="B208" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C208">
         <v>1.111569230769231E-9</v>
@@ -2951,7 +2948,7 @@
         <v>75</v>
       </c>
       <c r="B209" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C209">
         <v>1.111569230769231E-9</v>
@@ -2962,7 +2959,7 @@
         <v>75</v>
       </c>
       <c r="B210" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C210">
         <v>1.111569230769231E-9</v>
@@ -2973,7 +2970,7 @@
         <v>75</v>
       </c>
       <c r="B211" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C211">
         <v>1.111569230769231E-9</v>
@@ -2981,13 +2978,13 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B212" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C212">
-        <v>1.111569230769231E-9</v>
+        <v>2.8777846153846162E-9</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -2995,7 +2992,7 @@
         <v>76</v>
       </c>
       <c r="B213" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C213">
         <v>2.8777846153846162E-9</v>
@@ -3006,7 +3003,7 @@
         <v>76</v>
       </c>
       <c r="B214" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C214">
         <v>2.8777846153846162E-9</v>
@@ -3017,7 +3014,7 @@
         <v>76</v>
       </c>
       <c r="B215" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C215">
         <v>2.8777846153846162E-9</v>
@@ -3028,7 +3025,7 @@
         <v>76</v>
       </c>
       <c r="B216" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C216">
         <v>2.8777846153846162E-9</v>
@@ -3036,13 +3033,13 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B217" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C217">
-        <v>2.8777846153846162E-9</v>
+        <v>3.714576923076923E-9</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
@@ -3050,7 +3047,7 @@
         <v>77</v>
       </c>
       <c r="B218" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C218">
         <v>3.714576923076923E-9</v>
@@ -3061,7 +3058,7 @@
         <v>77</v>
       </c>
       <c r="B219" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C219">
         <v>3.714576923076923E-9</v>
@@ -3072,7 +3069,7 @@
         <v>77</v>
       </c>
       <c r="B220" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C220">
         <v>3.714576923076923E-9</v>
@@ -3083,7 +3080,7 @@
         <v>77</v>
       </c>
       <c r="B221" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C221">
         <v>3.714576923076923E-9</v>
@@ -3091,24 +3088,24 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B222" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C222">
-        <v>3.714576923076923E-9</v>
+        <v>1.969753846153846E-9</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B223" t="s">
         <v>41</v>
       </c>
       <c r="C223">
-        <v>1.969753846153846E-9</v>
+        <v>5.418069230769231E-9</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
@@ -3116,7 +3113,7 @@
         <v>79</v>
       </c>
       <c r="B224" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C224">
         <v>5.418069230769231E-9</v>
@@ -3127,7 +3124,7 @@
         <v>79</v>
       </c>
       <c r="B225" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C225">
         <v>5.418069230769231E-9</v>
@@ -3138,7 +3135,7 @@
         <v>79</v>
       </c>
       <c r="B226" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C226">
         <v>5.418069230769231E-9</v>
@@ -3149,20 +3146,9 @@
         <v>79</v>
       </c>
       <c r="B227" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C227">
-        <v>5.418069230769231E-9</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A228" t="s">
-        <v>79</v>
-      </c>
-      <c r="B228" t="s">
-        <v>82</v>
-      </c>
-      <c r="C228">
         <v>5.418069230769231E-9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow name should contain "lake", not "lakes"
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1708E204-E421-4F5C-9C25-D14AA61620AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497889A9-D9DB-4E55-B434-51D5C3F33E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
     <t>soil::industrial</t>
   </si>
   <si>
-    <t>Occupation, lakes, artificial</t>
+    <t>Occupation, lake, artificial</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Modify CFs in `dev\aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx`
Highlight only, do not change:
- "Occupation, forest, intesive" = 6.15385E-13 [leave the higher CF following precautionary principle, see 03e66ef1e3425d]

Add:
- "Occupation, lake, artificial" (natural resource::land) = 7.69231E-13, see 6596de1ceb
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1512D2-686E-41AC-A6EE-795D37BCBEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E687AF-FBBC-4D73-BEC4-D0D6743B2E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="91">
   <si>
     <t>name</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>soil::industrial</t>
+  </si>
+  <si>
+    <t>Occupation, lake, artificial</t>
   </si>
 </sst>
 </file>
@@ -318,12 +321,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -338,9 +347,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +794,7 @@
       <c r="B14" t="s">
         <v>80</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>6.1538461538461536E-13</v>
       </c>
     </row>
@@ -965,30 +975,30 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
+      <c r="A31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="2">
+        <v>7.6923076923076923E-13</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>80</v>
       </c>
       <c r="C32">
-        <v>7.3076923076923074E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>80</v>
@@ -999,7 +1009,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>80</v>
@@ -1010,7 +1020,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>80</v>
@@ -1021,7 +1031,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>80</v>
@@ -1032,7 +1042,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>80</v>
@@ -1043,7 +1053,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>80</v>
@@ -1054,13 +1064,13 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C39">
-        <v>4.1538461538461543E-12</v>
+        <v>7.3076923076923074E-13</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1068,7 +1078,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>4.1538461538461543E-12</v>
@@ -1079,7 +1089,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <v>4.1538461538461543E-12</v>
@@ -1090,7 +1100,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42">
         <v>4.1538461538461543E-12</v>
@@ -1101,7 +1111,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C43">
         <v>4.1538461538461543E-12</v>
@@ -1109,13 +1119,13 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C44">
-        <v>2.8661538461538461E-12</v>
+        <v>4.1538461538461543E-12</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1123,7 +1133,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>2.8661538461538461E-12</v>
@@ -1134,7 +1144,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46">
         <v>2.8661538461538461E-12</v>
@@ -1145,7 +1155,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47">
         <v>2.8661538461538461E-12</v>
@@ -1156,7 +1166,7 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C48">
         <v>2.8661538461538461E-12</v>
@@ -1164,13 +1174,13 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C49">
-        <v>2.076923076923077E-13</v>
+        <v>2.8661538461538461E-12</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1178,7 +1188,7 @@
         <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C50">
         <v>2.076923076923077E-13</v>
@@ -1189,7 +1199,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C51">
         <v>2.076923076923077E-13</v>
@@ -1200,7 +1210,7 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52">
         <v>2.076923076923077E-13</v>
@@ -1211,7 +1221,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C53">
         <v>2.076923076923077E-13</v>
@@ -1219,10 +1229,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C54">
         <v>2.076923076923077E-13</v>
@@ -1233,7 +1243,7 @@
         <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C55">
         <v>2.076923076923077E-13</v>
@@ -1244,7 +1254,7 @@
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56">
         <v>2.076923076923077E-13</v>
@@ -1255,7 +1265,7 @@
         <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57">
         <v>2.076923076923077E-13</v>
@@ -1266,7 +1276,7 @@
         <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C58">
         <v>2.076923076923077E-13</v>
@@ -1277,7 +1287,7 @@
         <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C59">
         <v>2.076923076923077E-13</v>
@@ -1285,13 +1295,13 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C60">
-        <v>-2.076923076923077E-13</v>
+        <v>2.076923076923077E-13</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1299,7 +1309,7 @@
         <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C61">
         <v>-2.076923076923077E-13</v>
@@ -1310,7 +1320,7 @@
         <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62">
         <v>-2.076923076923077E-13</v>
@@ -1321,7 +1331,7 @@
         <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63">
         <v>-2.076923076923077E-13</v>
@@ -1329,13 +1339,13 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C64">
-        <v>6.1892307692307702E-11</v>
+        <v>-2.076923076923077E-13</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,7 +1353,7 @@
         <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C65">
         <v>6.1892307692307702E-11</v>
@@ -1354,7 +1364,7 @@
         <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66">
         <v>6.1892307692307702E-11</v>
@@ -1365,7 +1375,7 @@
         <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C67">
         <v>6.1892307692307702E-11</v>
@@ -1376,7 +1386,7 @@
         <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C68">
         <v>6.1892307692307702E-11</v>
@@ -1384,13 +1394,13 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C69">
-        <v>3.2171538461538461E-10</v>
+        <v>6.1892307692307702E-11</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1398,7 +1408,7 @@
         <v>48</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C70">
         <v>3.2171538461538461E-10</v>
@@ -1409,7 +1419,7 @@
         <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71">
         <v>3.2171538461538461E-10</v>
@@ -1420,7 +1430,7 @@
         <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72">
         <v>3.2171538461538461E-10</v>
@@ -1431,7 +1441,7 @@
         <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C73">
         <v>3.2171538461538461E-10</v>
@@ -1439,13 +1449,13 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C74">
-        <v>1.143969230769231E-9</v>
+        <v>3.2171538461538461E-10</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1453,7 +1463,7 @@
         <v>49</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C75">
         <v>1.143969230769231E-9</v>
@@ -1464,7 +1474,7 @@
         <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76">
         <v>1.143969230769231E-9</v>
@@ -1475,7 +1485,7 @@
         <v>49</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77">
         <v>1.143969230769231E-9</v>
@@ -1486,7 +1496,7 @@
         <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C78">
         <v>1.143969230769231E-9</v>
@@ -1494,13 +1504,13 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C79">
-        <v>1.3678615384615381E-9</v>
+        <v>1.143969230769231E-9</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1508,7 +1518,7 @@
         <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C80">
         <v>1.3678615384615381E-9</v>
@@ -1519,7 +1529,7 @@
         <v>50</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C81">
         <v>1.3678615384615381E-9</v>
@@ -1530,7 +1540,7 @@
         <v>50</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C82">
         <v>1.3678615384615381E-9</v>
@@ -1541,7 +1551,7 @@
         <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C83">
         <v>1.3678615384615381E-9</v>
@@ -1549,13 +1559,13 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C84">
-        <v>1.9481538461538459E-10</v>
+        <v>1.3678615384615381E-9</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -1563,7 +1573,7 @@
         <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C85">
         <v>1.9481538461538459E-10</v>
@@ -1574,7 +1584,7 @@
         <v>51</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C86">
         <v>1.9481538461538459E-10</v>
@@ -1585,7 +1595,7 @@
         <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C87">
         <v>1.9481538461538459E-10</v>
@@ -1596,7 +1606,7 @@
         <v>51</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C88">
         <v>1.9481538461538459E-10</v>
@@ -1604,13 +1614,13 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C89">
-        <v>3.4684615384615383E-11</v>
+        <v>1.9481538461538459E-10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -1618,7 +1628,7 @@
         <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C90">
         <v>3.4684615384615383E-11</v>
@@ -1629,7 +1639,7 @@
         <v>52</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C91">
         <v>3.4684615384615383E-11</v>
@@ -1640,7 +1650,7 @@
         <v>52</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C92">
         <v>3.4684615384615383E-11</v>
@@ -1651,7 +1661,7 @@
         <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C93">
         <v>3.4684615384615383E-11</v>
@@ -1659,13 +1669,13 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C94">
-        <v>1.9969615384615379E-9</v>
+        <v>3.4684615384615383E-11</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -1673,7 +1683,7 @@
         <v>53</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C95">
         <v>1.9969615384615379E-9</v>
@@ -1684,7 +1694,7 @@
         <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C96">
         <v>1.9969615384615379E-9</v>
@@ -1695,7 +1705,7 @@
         <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C97">
         <v>1.9969615384615379E-9</v>
@@ -1706,7 +1716,7 @@
         <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C98">
         <v>1.9969615384615379E-9</v>
@@ -1714,13 +1724,13 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C99">
-        <v>4.8703846153846161E-10</v>
+        <v>1.9969615384615379E-9</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -1728,7 +1738,7 @@
         <v>54</v>
       </c>
       <c r="B100" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C100">
         <v>4.8703846153846161E-10</v>
@@ -1739,7 +1749,7 @@
         <v>54</v>
       </c>
       <c r="B101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C101">
         <v>4.8703846153846161E-10</v>
@@ -1750,7 +1760,7 @@
         <v>54</v>
       </c>
       <c r="B102" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C102">
         <v>4.8703846153846161E-10</v>
@@ -1761,7 +1771,7 @@
         <v>54</v>
       </c>
       <c r="B103" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C103">
         <v>4.8703846153846161E-10</v>
@@ -1769,13 +1779,13 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C104">
-        <v>1.9938461538461541E-11</v>
+        <v>4.8703846153846161E-10</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -1783,7 +1793,7 @@
         <v>55</v>
       </c>
       <c r="B105" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C105">
         <v>1.9938461538461541E-11</v>
@@ -1794,7 +1804,7 @@
         <v>55</v>
       </c>
       <c r="B106" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C106">
         <v>1.9938461538461541E-11</v>
@@ -1805,7 +1815,7 @@
         <v>55</v>
       </c>
       <c r="B107" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C107">
         <v>1.9938461538461541E-11</v>
@@ -1816,7 +1826,7 @@
         <v>55</v>
       </c>
       <c r="B108" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C108">
         <v>1.9938461538461541E-11</v>
@@ -1824,13 +1834,13 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C109">
-        <v>1.3188461538461541E-10</v>
+        <v>1.9938461538461541E-11</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -1838,7 +1848,7 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C110">
         <v>1.3188461538461541E-10</v>
@@ -1849,7 +1859,7 @@
         <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C111">
         <v>1.3188461538461541E-10</v>
@@ -1860,7 +1870,7 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C112">
         <v>1.3188461538461541E-10</v>
@@ -1871,7 +1881,7 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C113">
         <v>1.3188461538461541E-10</v>
@@ -1879,13 +1889,13 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C114">
-        <v>1.7687076923076921E-9</v>
+        <v>1.3188461538461541E-10</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -1893,7 +1903,7 @@
         <v>57</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C115">
         <v>1.7687076923076921E-9</v>
@@ -1904,7 +1914,7 @@
         <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C116">
         <v>1.7687076923076921E-9</v>
@@ -1915,7 +1925,7 @@
         <v>57</v>
       </c>
       <c r="B117" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C117">
         <v>1.7687076923076921E-9</v>
@@ -1926,7 +1936,7 @@
         <v>57</v>
       </c>
       <c r="B118" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C118">
         <v>1.7687076923076921E-9</v>
@@ -1934,13 +1944,13 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C119">
-        <v>2.5629230769230769E-9</v>
+        <v>1.7687076923076921E-9</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -1948,7 +1958,7 @@
         <v>58</v>
       </c>
       <c r="B120" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C120">
         <v>2.5629230769230769E-9</v>
@@ -1959,7 +1969,7 @@
         <v>58</v>
       </c>
       <c r="B121" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C121">
         <v>2.5629230769230769E-9</v>
@@ -1970,7 +1980,7 @@
         <v>58</v>
       </c>
       <c r="B122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C122">
         <v>2.5629230769230769E-9</v>
@@ -1981,7 +1991,7 @@
         <v>58</v>
       </c>
       <c r="B123" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C123">
         <v>2.5629230769230769E-9</v>
@@ -1989,13 +1999,13 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B124" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C124">
-        <v>7.6659230769230773E-10</v>
+        <v>2.5629230769230769E-9</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2003,7 +2013,7 @@
         <v>59</v>
       </c>
       <c r="B125" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C125">
         <v>7.6659230769230773E-10</v>
@@ -2014,7 +2024,7 @@
         <v>59</v>
       </c>
       <c r="B126" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C126">
         <v>7.6659230769230773E-10</v>
@@ -2025,7 +2035,7 @@
         <v>59</v>
       </c>
       <c r="B127" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C127">
         <v>7.6659230769230773E-10</v>
@@ -2036,7 +2046,7 @@
         <v>59</v>
       </c>
       <c r="B128" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C128">
         <v>7.6659230769230773E-10</v>
@@ -2044,24 +2054,24 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="B129" t="s">
         <v>82</v>
       </c>
       <c r="C129">
-        <v>7.4769230769230768E-12</v>
+        <v>7.6659230769230773E-10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B130" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C130">
-        <v>6.2307692307692306E-13</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -2069,7 +2079,7 @@
         <v>60</v>
       </c>
       <c r="B131" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C131">
         <v>6.2307692307692306E-13</v>
@@ -2080,7 +2090,7 @@
         <v>60</v>
       </c>
       <c r="B132" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C132">
         <v>6.2307692307692306E-13</v>
@@ -2091,7 +2101,7 @@
         <v>60</v>
       </c>
       <c r="B133" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C133">
         <v>6.2307692307692306E-13</v>
@@ -2102,7 +2112,7 @@
         <v>60</v>
       </c>
       <c r="B134" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C134">
         <v>6.2307692307692306E-13</v>
@@ -2110,13 +2120,13 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B135" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C135">
-        <v>4.29923076923077E-10</v>
+        <v>6.2307692307692306E-13</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -2124,7 +2134,7 @@
         <v>61</v>
       </c>
       <c r="B136" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C136">
         <v>4.29923076923077E-10</v>
@@ -2135,7 +2145,7 @@
         <v>61</v>
       </c>
       <c r="B137" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C137">
         <v>4.29923076923077E-10</v>
@@ -2146,7 +2156,7 @@
         <v>61</v>
       </c>
       <c r="B138" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C138">
         <v>4.29923076923077E-10</v>
@@ -2157,7 +2167,7 @@
         <v>61</v>
       </c>
       <c r="B139" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C139">
         <v>4.29923076923077E-10</v>
@@ -2165,13 +2175,13 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B140" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C140">
-        <v>1.4858307692307699E-9</v>
+        <v>4.29923076923077E-10</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -2179,7 +2189,7 @@
         <v>62</v>
       </c>
       <c r="B141" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C141">
         <v>1.4858307692307699E-9</v>
@@ -2190,7 +2200,7 @@
         <v>62</v>
       </c>
       <c r="B142" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C142">
         <v>1.4858307692307699E-9</v>
@@ -2201,7 +2211,7 @@
         <v>62</v>
       </c>
       <c r="B143" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C143">
         <v>1.4858307692307699E-9</v>
@@ -2212,7 +2222,7 @@
         <v>62</v>
       </c>
       <c r="B144" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C144">
         <v>1.4858307692307699E-9</v>
@@ -2220,13 +2230,13 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B145" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C145">
-        <v>4.3740000000000001E-10</v>
+        <v>1.4858307692307699E-9</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -2234,7 +2244,7 @@
         <v>63</v>
       </c>
       <c r="B146" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C146">
         <v>4.3740000000000001E-10</v>
@@ -2245,7 +2255,7 @@
         <v>63</v>
       </c>
       <c r="B147" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C147">
         <v>4.3740000000000001E-10</v>
@@ -2256,7 +2266,7 @@
         <v>63</v>
       </c>
       <c r="B148" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C148">
         <v>4.3740000000000001E-10</v>
@@ -2267,7 +2277,7 @@
         <v>63</v>
       </c>
       <c r="B149" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C149">
         <v>4.3740000000000001E-10</v>
@@ -2275,13 +2285,13 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B150" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C150">
-        <v>3.2090538461538469E-9</v>
+        <v>4.3740000000000001E-10</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -2289,7 +2299,7 @@
         <v>64</v>
       </c>
       <c r="B151" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C151">
         <v>3.2090538461538469E-9</v>
@@ -2300,7 +2310,7 @@
         <v>64</v>
       </c>
       <c r="B152" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C152">
         <v>3.2090538461538469E-9</v>
@@ -2311,7 +2321,7 @@
         <v>64</v>
       </c>
       <c r="B153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C153">
         <v>3.2090538461538469E-9</v>
@@ -2322,7 +2332,7 @@
         <v>64</v>
       </c>
       <c r="B154" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C154">
         <v>3.2090538461538469E-9</v>
@@ -2330,13 +2340,13 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B155" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C155">
-        <v>2.2846153846153851E-12</v>
+        <v>3.2090538461538469E-9</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -2344,7 +2354,7 @@
         <v>65</v>
       </c>
       <c r="B156" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C156">
         <v>2.2846153846153851E-12</v>
@@ -2355,7 +2365,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C157">
         <v>2.2846153846153851E-12</v>
@@ -2366,7 +2376,7 @@
         <v>65</v>
       </c>
       <c r="B158" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C158">
         <v>2.2846153846153851E-12</v>
@@ -2377,7 +2387,7 @@
         <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C159">
         <v>2.2846153846153851E-12</v>
@@ -2385,13 +2395,13 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B160" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C160">
-        <v>2.3982230769230768E-9</v>
+        <v>2.2846153846153851E-12</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -2399,7 +2409,7 @@
         <v>66</v>
       </c>
       <c r="B161" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C161">
         <v>2.3982230769230768E-9</v>
@@ -2410,7 +2420,7 @@
         <v>66</v>
       </c>
       <c r="B162" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C162">
         <v>2.3982230769230768E-9</v>
@@ -2421,7 +2431,7 @@
         <v>66</v>
       </c>
       <c r="B163" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C163">
         <v>2.3982230769230768E-9</v>
@@ -2432,7 +2442,7 @@
         <v>66</v>
       </c>
       <c r="B164" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C164">
         <v>2.3982230769230768E-9</v>
@@ -2440,13 +2450,13 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B165" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C165">
-        <v>3.7176923076923081E-11</v>
+        <v>2.3982230769230768E-9</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -2454,7 +2464,7 @@
         <v>67</v>
       </c>
       <c r="B166" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C166">
         <v>3.7176923076923081E-11</v>
@@ -2465,7 +2475,7 @@
         <v>67</v>
       </c>
       <c r="B167" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C167">
         <v>3.7176923076923081E-11</v>
@@ -2476,7 +2486,7 @@
         <v>67</v>
       </c>
       <c r="B168" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C168">
         <v>3.7176923076923081E-11</v>
@@ -2487,7 +2497,7 @@
         <v>67</v>
       </c>
       <c r="B169" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C169">
         <v>3.7176923076923081E-11</v>
@@ -2495,13 +2505,13 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B170" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C170">
-        <v>1.6968461538461539E-10</v>
+        <v>3.7176923076923081E-11</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -2509,7 +2519,7 @@
         <v>68</v>
       </c>
       <c r="B171" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C171">
         <v>1.6968461538461539E-10</v>
@@ -2520,7 +2530,7 @@
         <v>68</v>
       </c>
       <c r="B172" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C172">
         <v>1.6968461538461539E-10</v>
@@ -2531,7 +2541,7 @@
         <v>68</v>
       </c>
       <c r="B173" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C173">
         <v>1.6968461538461539E-10</v>
@@ -2542,7 +2552,7 @@
         <v>68</v>
       </c>
       <c r="B174" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C174">
         <v>1.6968461538461539E-10</v>
@@ -2550,13 +2560,13 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B175" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C175">
-        <v>7.4769230769230768E-12</v>
+        <v>1.6968461538461539E-10</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -2564,7 +2574,7 @@
         <v>69</v>
       </c>
       <c r="B176" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C176">
         <v>7.4769230769230768E-12</v>
@@ -2575,7 +2585,7 @@
         <v>69</v>
       </c>
       <c r="B177" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C177">
         <v>7.4769230769230768E-12</v>
@@ -2586,7 +2596,7 @@
         <v>69</v>
       </c>
       <c r="B178" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C178">
         <v>7.4769230769230768E-12</v>
@@ -2597,7 +2607,7 @@
         <v>69</v>
       </c>
       <c r="B179" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C179">
         <v>7.4769230769230768E-12</v>
@@ -2605,13 +2615,13 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B180" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C180">
-        <v>7.0615384615384616E-12</v>
+        <v>7.4769230769230768E-12</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -2619,7 +2629,7 @@
         <v>70</v>
       </c>
       <c r="B181" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C181">
         <v>7.0615384615384616E-12</v>
@@ -2630,7 +2640,7 @@
         <v>70</v>
       </c>
       <c r="B182" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C182">
         <v>7.0615384615384616E-12</v>
@@ -2641,7 +2651,7 @@
         <v>70</v>
       </c>
       <c r="B183" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C183">
         <v>7.0615384615384616E-12</v>
@@ -2652,7 +2662,7 @@
         <v>70</v>
       </c>
       <c r="B184" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C184">
         <v>7.0615384615384616E-12</v>
@@ -2663,7 +2673,7 @@
         <v>70</v>
       </c>
       <c r="B185" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C185">
         <v>7.0615384615384616E-12</v>
@@ -2671,13 +2681,13 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B186" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C186">
-        <v>3.1153846153846161E-12</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -2685,7 +2695,7 @@
         <v>71</v>
       </c>
       <c r="B187" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C187">
         <v>3.1153846153846161E-12</v>
@@ -2696,7 +2706,7 @@
         <v>71</v>
       </c>
       <c r="B188" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C188">
         <v>3.1153846153846161E-12</v>
@@ -2707,7 +2717,7 @@
         <v>71</v>
       </c>
       <c r="B189" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C189">
         <v>3.1153846153846161E-12</v>
@@ -2718,7 +2728,7 @@
         <v>71</v>
       </c>
       <c r="B190" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C190">
         <v>3.1153846153846161E-12</v>
@@ -2726,13 +2736,13 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B191" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C191">
-        <v>7.0615384615384616E-12</v>
+        <v>3.1153846153846161E-12</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -2740,7 +2750,7 @@
         <v>72</v>
       </c>
       <c r="B192" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C192">
         <v>7.0615384615384616E-12</v>
@@ -2751,7 +2761,7 @@
         <v>72</v>
       </c>
       <c r="B193" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C193">
         <v>7.0615384615384616E-12</v>
@@ -2762,7 +2772,7 @@
         <v>72</v>
       </c>
       <c r="B194" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C194">
         <v>7.0615384615384616E-12</v>
@@ -2773,7 +2783,7 @@
         <v>72</v>
       </c>
       <c r="B195" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C195">
         <v>7.0615384615384616E-12</v>
@@ -2781,13 +2791,13 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B196" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C196">
-        <v>4.1933076923076919E-10</v>
+        <v>7.0615384615384616E-12</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -2795,7 +2805,7 @@
         <v>73</v>
       </c>
       <c r="B197" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C197">
         <v>4.1933076923076919E-10</v>
@@ -2806,7 +2816,7 @@
         <v>73</v>
       </c>
       <c r="B198" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C198">
         <v>4.1933076923076919E-10</v>
@@ -2817,7 +2827,7 @@
         <v>73</v>
       </c>
       <c r="B199" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C199">
         <v>4.1933076923076919E-10</v>
@@ -2828,7 +2838,7 @@
         <v>73</v>
       </c>
       <c r="B200" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C200">
         <v>4.1933076923076919E-10</v>
@@ -2836,13 +2846,13 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B201" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C201">
-        <v>1.5263307692307689E-9</v>
+        <v>4.1933076923076919E-10</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -2850,7 +2860,7 @@
         <v>74</v>
       </c>
       <c r="B202" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C202">
         <v>1.5263307692307689E-9</v>
@@ -2861,7 +2871,7 @@
         <v>74</v>
       </c>
       <c r="B203" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C203">
         <v>1.5263307692307689E-9</v>
@@ -2872,7 +2882,7 @@
         <v>74</v>
       </c>
       <c r="B204" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C204">
         <v>1.5263307692307689E-9</v>
@@ -2883,7 +2893,7 @@
         <v>74</v>
       </c>
       <c r="B205" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C205">
         <v>1.5263307692307689E-9</v>
@@ -2891,13 +2901,13 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B206" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C206">
-        <v>1.111569230769231E-9</v>
+        <v>1.5263307692307689E-9</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
@@ -2905,7 +2915,7 @@
         <v>75</v>
       </c>
       <c r="B207" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C207">
         <v>1.111569230769231E-9</v>
@@ -2916,7 +2926,7 @@
         <v>75</v>
       </c>
       <c r="B208" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C208">
         <v>1.111569230769231E-9</v>
@@ -2927,7 +2937,7 @@
         <v>75</v>
       </c>
       <c r="B209" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C209">
         <v>1.111569230769231E-9</v>
@@ -2938,7 +2948,7 @@
         <v>75</v>
       </c>
       <c r="B210" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C210">
         <v>1.111569230769231E-9</v>
@@ -2946,13 +2956,13 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B211" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C211">
-        <v>2.8777846153846162E-9</v>
+        <v>1.111569230769231E-9</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -2960,7 +2970,7 @@
         <v>76</v>
       </c>
       <c r="B212" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C212">
         <v>2.8777846153846162E-9</v>
@@ -2971,7 +2981,7 @@
         <v>76</v>
       </c>
       <c r="B213" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C213">
         <v>2.8777846153846162E-9</v>
@@ -2982,7 +2992,7 @@
         <v>76</v>
       </c>
       <c r="B214" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C214">
         <v>2.8777846153846162E-9</v>
@@ -2993,7 +3003,7 @@
         <v>76</v>
       </c>
       <c r="B215" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C215">
         <v>2.8777846153846162E-9</v>
@@ -3001,13 +3011,13 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B216" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C216">
-        <v>3.714576923076923E-9</v>
+        <v>2.8777846153846162E-9</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -3015,7 +3025,7 @@
         <v>77</v>
       </c>
       <c r="B217" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C217">
         <v>3.714576923076923E-9</v>
@@ -3026,7 +3036,7 @@
         <v>77</v>
       </c>
       <c r="B218" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C218">
         <v>3.714576923076923E-9</v>
@@ -3037,7 +3047,7 @@
         <v>77</v>
       </c>
       <c r="B219" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C219">
         <v>3.714576923076923E-9</v>
@@ -3048,7 +3058,7 @@
         <v>77</v>
       </c>
       <c r="B220" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C220">
         <v>3.714576923076923E-9</v>
@@ -3056,24 +3066,24 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B221" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C221">
-        <v>1.969753846153846E-9</v>
+        <v>3.714576923076923E-9</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B222" t="s">
         <v>41</v>
       </c>
       <c r="C222">
-        <v>5.418069230769231E-9</v>
+        <v>1.969753846153846E-9</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
@@ -3081,7 +3091,7 @@
         <v>79</v>
       </c>
       <c r="B223" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C223">
         <v>5.418069230769231E-9</v>
@@ -3092,7 +3102,7 @@
         <v>79</v>
       </c>
       <c r="B224" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C224">
         <v>5.418069230769231E-9</v>
@@ -3103,7 +3113,7 @@
         <v>79</v>
       </c>
       <c r="B225" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C225">
         <v>5.418069230769231E-9</v>
@@ -3114,9 +3124,20 @@
         <v>79</v>
       </c>
       <c r="B226" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C226">
+        <v>5.418069230769231E-9</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>79</v>
+      </c>
+      <c r="B227" t="s">
+        <v>82</v>
+      </c>
+      <c r="C227">
         <v>5.418069230769231E-9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make CBI PB as in simapro
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
+++ b/src/aesa_pbs/data/aesa_ChangeBiosphereIntegrity_FunctionalDiversity_Hierarchist.xlsx
@@ -8,17 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E687AF-FBBC-4D73-BEC4-D0D6743B2E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497889A9-D9DB-4E55-B434-51D5C3F33E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -633,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,6 +652,7 @@
     <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -795,7 +806,7 @@
         <v>80</v>
       </c>
       <c r="C14" s="2">
-        <v>6.1538461538461536E-13</v>
+        <v>3.8461538461538462E-13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>